<commit_message>
One-click update from Van Paper 07:29 AM on 2025-08-28
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -949,7 +949,9 @@
       <x:c r="C33" s="9" t="s">
         <x:v>34</x:v>
       </x:c>
-      <x:c r="D33" s="13"/>
+      <x:c r="D33" s="12" t="n">
+        <x:v>45896</x:v>
+      </x:c>
       <x:c r="E33" s="9" t="s">
         <x:v>82</x:v>
       </x:c>

</xml_diff>

<commit_message>
One-click update from Van Paper 10:01 AM on 2025-08-28
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -266,6 +266,12 @@
   </x:si>
   <x:si>
     <x:t>0008277</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Las Americas </x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008279</x:t>
   </x:si>
   <x:si>
     <x:t>VALLEY OFFICE PARK</x:t>
@@ -381,7 +387,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:F38"/>
+  <x:dimension ref="A1:F39"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -977,32 +983,28 @@
       <x:c r="A35" s="9" t="s">
         <x:v>85</x:v>
       </x:c>
-      <x:c r="B35" s="9" t="s">
-        <x:v>30</x:v>
-      </x:c>
+      <x:c r="B35" s="13"/>
       <x:c r="C35" s="9" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D35" s="13"/>
+      <x:c r="E35" s="9" t="s">
         <x:v>86</x:v>
-      </x:c>
-      <x:c r="D35" s="12" t="n">
-        <x:v>45847</x:v>
-      </x:c>
-      <x:c r="E35" s="9" t="s">
-        <x:v>87</x:v>
       </x:c>
       <x:c r="F35"/>
     </x:row>
     <x:row r="36" ht="13.05" customHeight="1">
       <x:c r="A36" s="9" t="s">
+        <x:v>87</x:v>
+      </x:c>
+      <x:c r="B36" s="9" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C36" s="9" t="s">
         <x:v>88</x:v>
       </x:c>
-      <x:c r="B36" s="9" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C36" s="9" t="s">
-        <x:v>51</x:v>
-      </x:c>
       <x:c r="D36" s="12" t="n">
-        <x:v>45888</x:v>
+        <x:v>45847</x:v>
       </x:c>
       <x:c r="E36" s="9" t="s">
         <x:v>89</x:v>
@@ -1017,10 +1019,10 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="C37" s="9" t="s">
-        <x:v>34</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="D37" s="12" t="n">
-        <x:v>45848</x:v>
+        <x:v>45888</x:v>
       </x:c>
       <x:c r="E37" s="9" t="s">
         <x:v>91</x:v>
@@ -1032,18 +1034,36 @@
         <x:v>92</x:v>
       </x:c>
       <x:c r="B38" s="9" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="C38" s="9" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D38" s="12" t="n">
+        <x:v>45848</x:v>
+      </x:c>
+      <x:c r="E38" s="9" t="s">
         <x:v>93</x:v>
       </x:c>
-      <x:c r="C38" s="9" t="s">
+      <x:c r="F38"/>
+    </x:row>
+    <x:row r="39" ht="13.05" customHeight="1">
+      <x:c r="A39" s="9" t="s">
+        <x:v>94</x:v>
+      </x:c>
+      <x:c r="B39" s="9" t="s">
+        <x:v>95</x:v>
+      </x:c>
+      <x:c r="C39" s="9" t="s">
         <x:v>51</x:v>
       </x:c>
-      <x:c r="D38" s="12" t="n">
+      <x:c r="D39" s="12" t="n">
         <x:v>45895</x:v>
       </x:c>
-      <x:c r="E38" s="9" t="s">
-        <x:v>94</x:v>
-      </x:c>
-      <x:c r="F38"/>
+      <x:c r="E39" s="9" t="s">
+        <x:v>96</x:v>
+      </x:c>
+      <x:c r="F39"/>
     </x:row>
   </x:sheetData>
   <x:pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
One-click update from Van Paper 01:03 PM on 2025-09-02
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -272,6 +272,12 @@
   </x:si>
   <x:si>
     <x:t>0008279</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">BEIRUT LEBANESE STREET FOOD </x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008282</x:t>
   </x:si>
   <x:si>
     <x:t>VALLEY OFFICE PARK</x:t>
@@ -387,7 +393,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:F39"/>
+  <x:dimension ref="A1:F40"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -998,31 +1004,29 @@
         <x:v>87</x:v>
       </x:c>
       <x:c r="B36" s="9" t="s">
-        <x:v>30</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="C36" s="9" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D36" s="13"/>
+      <x:c r="E36" s="9" t="s">
         <x:v>88</x:v>
-      </x:c>
-      <x:c r="D36" s="12" t="n">
-        <x:v>45847</x:v>
-      </x:c>
-      <x:c r="E36" s="9" t="s">
-        <x:v>89</x:v>
       </x:c>
       <x:c r="F36"/>
     </x:row>
     <x:row r="37" ht="13.05" customHeight="1">
       <x:c r="A37" s="9" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="B37" s="9" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C37" s="9" t="s">
         <x:v>90</x:v>
       </x:c>
-      <x:c r="B37" s="9" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C37" s="9" t="s">
-        <x:v>51</x:v>
-      </x:c>
       <x:c r="D37" s="12" t="n">
-        <x:v>45888</x:v>
+        <x:v>45847</x:v>
       </x:c>
       <x:c r="E37" s="9" t="s">
         <x:v>91</x:v>
@@ -1037,10 +1041,10 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="C38" s="9" t="s">
-        <x:v>34</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="D38" s="12" t="n">
-        <x:v>45848</x:v>
+        <x:v>45888</x:v>
       </x:c>
       <x:c r="E38" s="9" t="s">
         <x:v>93</x:v>
@@ -1052,18 +1056,36 @@
         <x:v>94</x:v>
       </x:c>
       <x:c r="B39" s="9" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="C39" s="9" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D39" s="12" t="n">
+        <x:v>45848</x:v>
+      </x:c>
+      <x:c r="E39" s="9" t="s">
         <x:v>95</x:v>
       </x:c>
-      <x:c r="C39" s="9" t="s">
+      <x:c r="F39"/>
+    </x:row>
+    <x:row r="40" ht="13.05" customHeight="1">
+      <x:c r="A40" s="9" t="s">
+        <x:v>96</x:v>
+      </x:c>
+      <x:c r="B40" s="9" t="s">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="C40" s="9" t="s">
         <x:v>51</x:v>
       </x:c>
-      <x:c r="D39" s="12" t="n">
+      <x:c r="D40" s="12" t="n">
         <x:v>45895</x:v>
       </x:c>
-      <x:c r="E39" s="9" t="s">
-        <x:v>96</x:v>
-      </x:c>
-      <x:c r="F39"/>
+      <x:c r="E40" s="9" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="F40"/>
     </x:row>
   </x:sheetData>
   <x:pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
One-click update from Van Paper 08:21 AM on 2025-09-04
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -278,6 +278,12 @@
   </x:si>
   <x:si>
     <x:t>0008282</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Olivers</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008284</x:t>
   </x:si>
   <x:si>
     <x:t>VALLEY OFFICE PARK</x:t>
@@ -393,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:F40"/>
+  <x:dimension ref="A1:F41"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -1020,31 +1026,29 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B37" s="9" t="s">
-        <x:v>30</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="C37" s="9" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D37" s="13"/>
+      <x:c r="E37" s="9" t="s">
         <x:v>90</x:v>
-      </x:c>
-      <x:c r="D37" s="12" t="n">
-        <x:v>45847</x:v>
-      </x:c>
-      <x:c r="E37" s="9" t="s">
-        <x:v>91</x:v>
       </x:c>
       <x:c r="F37"/>
     </x:row>
     <x:row r="38" ht="13.05" customHeight="1">
       <x:c r="A38" s="9" t="s">
+        <x:v>91</x:v>
+      </x:c>
+      <x:c r="B38" s="9" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C38" s="9" t="s">
         <x:v>92</x:v>
       </x:c>
-      <x:c r="B38" s="9" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C38" s="9" t="s">
-        <x:v>51</x:v>
-      </x:c>
       <x:c r="D38" s="12" t="n">
-        <x:v>45888</x:v>
+        <x:v>45847</x:v>
       </x:c>
       <x:c r="E38" s="9" t="s">
         <x:v>93</x:v>
@@ -1059,10 +1063,10 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="C39" s="9" t="s">
-        <x:v>34</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="D39" s="12" t="n">
-        <x:v>45848</x:v>
+        <x:v>45888</x:v>
       </x:c>
       <x:c r="E39" s="9" t="s">
         <x:v>95</x:v>
@@ -1074,18 +1078,36 @@
         <x:v>96</x:v>
       </x:c>
       <x:c r="B40" s="9" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="C40" s="9" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D40" s="12" t="n">
+        <x:v>45848</x:v>
+      </x:c>
+      <x:c r="E40" s="9" t="s">
         <x:v>97</x:v>
       </x:c>
-      <x:c r="C40" s="9" t="s">
+      <x:c r="F40"/>
+    </x:row>
+    <x:row r="41" ht="13.05" customHeight="1">
+      <x:c r="A41" s="9" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="B41" s="9" t="s">
+        <x:v>99</x:v>
+      </x:c>
+      <x:c r="C41" s="9" t="s">
         <x:v>51</x:v>
       </x:c>
-      <x:c r="D40" s="12" t="n">
+      <x:c r="D41" s="12" t="n">
         <x:v>45895</x:v>
       </x:c>
-      <x:c r="E40" s="9" t="s">
-        <x:v>98</x:v>
-      </x:c>
-      <x:c r="F40"/>
+      <x:c r="E41" s="9" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="F41"/>
     </x:row>
   </x:sheetData>
   <x:pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
One-click update from Van Paper 08:23 AM on 2025-09-09
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -238,7 +238,7 @@
     <x:t>0008264</x:t>
   </x:si>
   <x:si>
-    <x:t>The Bellows Bistro</x:t>
+    <x:t>THE BELLOWS BISTRO</x:t>
   </x:si>
   <x:si>
     <x:t>0008268</x:t>
@@ -917,7 +917,7 @@
         <x:v>17</x:v>
       </x:c>
       <x:c r="C30" s="9" t="s">
-        <x:v>7</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="D30" s="13"/>
       <x:c r="E30" s="9" t="s">

</xml_diff>

<commit_message>
One-click update from Van Paper 09:20 AM on 2025-09-11
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -244,7 +244,7 @@
     <x:t>0008268</x:t>
   </x:si>
   <x:si>
-    <x:t>Chaska Market</x:t>
+    <x:t>CHASKA MARKET</x:t>
   </x:si>
   <x:si>
     <x:t>0008270</x:t>
@@ -919,7 +919,9 @@
       <x:c r="C30" s="9" t="s">
         <x:v>34</x:v>
       </x:c>
-      <x:c r="D30" s="13"/>
+      <x:c r="D30" s="12" t="n">
+        <x:v>45910</x:v>
+      </x:c>
       <x:c r="E30" s="9" t="s">
         <x:v>76</x:v>
       </x:c>

</xml_diff>

<commit_message>
One-click update from Van Paper 07:55 AM on 2025-09-12
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -205,7 +205,7 @@
     <x:t>0008241</x:t>
   </x:si>
   <x:si>
-    <x:t>Mr Mustacheo</x:t>
+    <x:t>MR. MUSTACHEO GROUP LLC</x:t>
   </x:si>
   <x:si>
     <x:t>0008242</x:t>
@@ -835,9 +835,11 @@
         <x:v>33</x:v>
       </x:c>
       <x:c r="C25" s="9" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="D25" s="13"/>
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D25" s="12" t="n">
+        <x:v>45911</x:v>
+      </x:c>
       <x:c r="E25" s="9" t="s">
         <x:v>65</x:v>
       </x:c>
@@ -937,7 +939,9 @@
       <x:c r="C31" s="9" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="D31" s="13"/>
+      <x:c r="D31" s="12" t="n">
+        <x:v>45911</x:v>
+      </x:c>
       <x:c r="E31" s="9" t="s">
         <x:v>78</x:v>
       </x:c>

</xml_diff>

<commit_message>
One-click update from Van Paper 01:03 PM on 2025-09-12
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -284,6 +284,12 @@
   </x:si>
   <x:si>
     <x:t>0008284</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Shakopee Brewhall</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008296</x:t>
   </x:si>
   <x:si>
     <x:t>VALLEY OFFICE PARK</x:t>
@@ -399,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:F41"/>
+  <x:dimension ref="A1:F42"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -1021,7 +1027,9 @@
       <x:c r="C36" s="9" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="D36" s="13"/>
+      <x:c r="D36" s="12" t="n">
+        <x:v>45912</x:v>
+      </x:c>
       <x:c r="E36" s="9" t="s">
         <x:v>88</x:v>
       </x:c>
@@ -1048,31 +1056,29 @@
         <x:v>91</x:v>
       </x:c>
       <x:c r="B38" s="9" t="s">
-        <x:v>30</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C38" s="9" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D38" s="13"/>
+      <x:c r="E38" s="9" t="s">
         <x:v>92</x:v>
-      </x:c>
-      <x:c r="D38" s="12" t="n">
-        <x:v>45847</x:v>
-      </x:c>
-      <x:c r="E38" s="9" t="s">
-        <x:v>93</x:v>
       </x:c>
       <x:c r="F38"/>
     </x:row>
     <x:row r="39" ht="13.05" customHeight="1">
       <x:c r="A39" s="9" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="B39" s="9" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C39" s="9" t="s">
         <x:v>94</x:v>
       </x:c>
-      <x:c r="B39" s="9" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C39" s="9" t="s">
-        <x:v>51</x:v>
-      </x:c>
       <x:c r="D39" s="12" t="n">
-        <x:v>45888</x:v>
+        <x:v>45847</x:v>
       </x:c>
       <x:c r="E39" s="9" t="s">
         <x:v>95</x:v>
@@ -1087,10 +1093,10 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="C40" s="9" t="s">
-        <x:v>34</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="D40" s="12" t="n">
-        <x:v>45848</x:v>
+        <x:v>45888</x:v>
       </x:c>
       <x:c r="E40" s="9" t="s">
         <x:v>97</x:v>
@@ -1102,18 +1108,36 @@
         <x:v>98</x:v>
       </x:c>
       <x:c r="B41" s="9" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="C41" s="9" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D41" s="12" t="n">
+        <x:v>45848</x:v>
+      </x:c>
+      <x:c r="E41" s="9" t="s">
         <x:v>99</x:v>
       </x:c>
-      <x:c r="C41" s="9" t="s">
+      <x:c r="F41"/>
+    </x:row>
+    <x:row r="42" ht="13.05" customHeight="1">
+      <x:c r="A42" s="9" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="B42" s="9" t="s">
+        <x:v>101</x:v>
+      </x:c>
+      <x:c r="C42" s="9" t="s">
         <x:v>51</x:v>
       </x:c>
-      <x:c r="D41" s="12" t="n">
+      <x:c r="D42" s="12" t="n">
         <x:v>45895</x:v>
       </x:c>
-      <x:c r="E41" s="9" t="s">
-        <x:v>100</x:v>
-      </x:c>
-      <x:c r="F41"/>
+      <x:c r="E42" s="9" t="s">
+        <x:v>102</x:v>
+      </x:c>
+      <x:c r="F42"/>
     </x:row>
   </x:sheetData>
   <x:pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
One-click update from Van Paper 08:11 AM on 2025-09-16
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -290,6 +290,12 @@
   </x:si>
   <x:si>
     <x:t>0008296</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TAQUERIA Y MERCADO ANDALE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008300</x:t>
   </x:si>
   <x:si>
     <x:t>VALLEY OFFICE PARK</x:t>
@@ -405,7 +411,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:F42"/>
+  <x:dimension ref="A1:F43"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -1072,31 +1078,29 @@
         <x:v>93</x:v>
       </x:c>
       <x:c r="B39" s="9" t="s">
-        <x:v>30</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="C39" s="9" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="D39" s="13"/>
+      <x:c r="E39" s="9" t="s">
         <x:v>94</x:v>
-      </x:c>
-      <x:c r="D39" s="12" t="n">
-        <x:v>45847</x:v>
-      </x:c>
-      <x:c r="E39" s="9" t="s">
-        <x:v>95</x:v>
       </x:c>
       <x:c r="F39"/>
     </x:row>
     <x:row r="40" ht="13.05" customHeight="1">
       <x:c r="A40" s="9" t="s">
+        <x:v>95</x:v>
+      </x:c>
+      <x:c r="B40" s="9" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C40" s="9" t="s">
         <x:v>96</x:v>
       </x:c>
-      <x:c r="B40" s="9" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C40" s="9" t="s">
-        <x:v>51</x:v>
-      </x:c>
       <x:c r="D40" s="12" t="n">
-        <x:v>45888</x:v>
+        <x:v>45847</x:v>
       </x:c>
       <x:c r="E40" s="9" t="s">
         <x:v>97</x:v>
@@ -1111,10 +1115,10 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="C41" s="9" t="s">
-        <x:v>34</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="D41" s="12" t="n">
-        <x:v>45848</x:v>
+        <x:v>45888</x:v>
       </x:c>
       <x:c r="E41" s="9" t="s">
         <x:v>99</x:v>
@@ -1126,18 +1130,36 @@
         <x:v>100</x:v>
       </x:c>
       <x:c r="B42" s="9" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="C42" s="9" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D42" s="12" t="n">
+        <x:v>45848</x:v>
+      </x:c>
+      <x:c r="E42" s="9" t="s">
         <x:v>101</x:v>
       </x:c>
-      <x:c r="C42" s="9" t="s">
+      <x:c r="F42"/>
+    </x:row>
+    <x:row r="43" ht="13.05" customHeight="1">
+      <x:c r="A43" s="9" t="s">
+        <x:v>102</x:v>
+      </x:c>
+      <x:c r="B43" s="9" t="s">
+        <x:v>103</x:v>
+      </x:c>
+      <x:c r="C43" s="9" t="s">
         <x:v>51</x:v>
       </x:c>
-      <x:c r="D42" s="12" t="n">
+      <x:c r="D43" s="12" t="n">
         <x:v>45895</x:v>
       </x:c>
-      <x:c r="E42" s="9" t="s">
-        <x:v>102</x:v>
-      </x:c>
-      <x:c r="F42"/>
+      <x:c r="E43" s="9" t="s">
+        <x:v>104</x:v>
+      </x:c>
+      <x:c r="F43"/>
     </x:row>
   </x:sheetData>
   <x:pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
One-click update from Van Paper 07:59 AM on 2025-09-17
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -296,6 +296,12 @@
   </x:si>
   <x:si>
     <x:t>0008300</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LITTLE BIRD DELICATESSEN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008303</x:t>
   </x:si>
   <x:si>
     <x:t>VALLEY OFFICE PARK</x:t>
@@ -411,7 +417,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:F43"/>
+  <x:dimension ref="A1:F44"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -1083,7 +1089,9 @@
       <x:c r="C39" s="9" t="s">
         <x:v>51</x:v>
       </x:c>
-      <x:c r="D39" s="13"/>
+      <x:c r="D39" s="12" t="n">
+        <x:v>45916</x:v>
+      </x:c>
       <x:c r="E39" s="9" t="s">
         <x:v>94</x:v>
       </x:c>
@@ -1094,31 +1102,29 @@
         <x:v>95</x:v>
       </x:c>
       <x:c r="B40" s="9" t="s">
-        <x:v>30</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="C40" s="9" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="D40" s="13"/>
+      <x:c r="E40" s="9" t="s">
         <x:v>96</x:v>
-      </x:c>
-      <x:c r="D40" s="12" t="n">
-        <x:v>45847</x:v>
-      </x:c>
-      <x:c r="E40" s="9" t="s">
-        <x:v>97</x:v>
       </x:c>
       <x:c r="F40"/>
     </x:row>
     <x:row r="41" ht="13.05" customHeight="1">
       <x:c r="A41" s="9" t="s">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="B41" s="9" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C41" s="9" t="s">
         <x:v>98</x:v>
       </x:c>
-      <x:c r="B41" s="9" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C41" s="9" t="s">
-        <x:v>51</x:v>
-      </x:c>
       <x:c r="D41" s="12" t="n">
-        <x:v>45888</x:v>
+        <x:v>45847</x:v>
       </x:c>
       <x:c r="E41" s="9" t="s">
         <x:v>99</x:v>
@@ -1133,10 +1139,10 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="C42" s="9" t="s">
-        <x:v>34</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="D42" s="12" t="n">
-        <x:v>45848</x:v>
+        <x:v>45888</x:v>
       </x:c>
       <x:c r="E42" s="9" t="s">
         <x:v>101</x:v>
@@ -1148,18 +1154,36 @@
         <x:v>102</x:v>
       </x:c>
       <x:c r="B43" s="9" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="C43" s="9" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D43" s="12" t="n">
+        <x:v>45848</x:v>
+      </x:c>
+      <x:c r="E43" s="9" t="s">
         <x:v>103</x:v>
       </x:c>
-      <x:c r="C43" s="9" t="s">
+      <x:c r="F43"/>
+    </x:row>
+    <x:row r="44" ht="13.05" customHeight="1">
+      <x:c r="A44" s="9" t="s">
+        <x:v>104</x:v>
+      </x:c>
+      <x:c r="B44" s="9" t="s">
+        <x:v>105</x:v>
+      </x:c>
+      <x:c r="C44" s="9" t="s">
         <x:v>51</x:v>
       </x:c>
-      <x:c r="D43" s="12" t="n">
+      <x:c r="D44" s="12" t="n">
         <x:v>45895</x:v>
       </x:c>
-      <x:c r="E43" s="9" t="s">
-        <x:v>104</x:v>
-      </x:c>
-      <x:c r="F43"/>
+      <x:c r="E44" s="9" t="s">
+        <x:v>106</x:v>
+      </x:c>
+      <x:c r="F44"/>
     </x:row>
   </x:sheetData>
   <x:pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
One-click update from Van Paper 08:15 AM on 2025-09-18
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -304,6 +304,15 @@
     <x:t>0008303</x:t>
   </x:si>
   <x:si>
+    <x:t>Fiesta Mexicana</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Zigan, Gerald L</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008306</x:t>
+  </x:si>
+  <x:si>
     <x:t>VALLEY OFFICE PARK</x:t>
   </x:si>
   <x:si>
@@ -326,9 +335,6 @@
   </x:si>
   <x:si>
     <x:t>BEAR COUNTRY MEATS LLC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Zigan, Gerald L</x:t>
   </x:si>
   <x:si>
     <x:t>0007429</x:t>
@@ -417,7 +423,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:F44"/>
+  <x:dimension ref="A1:F45"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -1118,14 +1124,12 @@
         <x:v>97</x:v>
       </x:c>
       <x:c r="B41" s="9" t="s">
-        <x:v>30</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="C41" s="9" t="s">
-        <x:v>98</x:v>
-      </x:c>
-      <x:c r="D41" s="12" t="n">
-        <x:v>45847</x:v>
-      </x:c>
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="D41" s="13"/>
       <x:c r="E41" s="9" t="s">
         <x:v>99</x:v>
       </x:c>
@@ -1136,57 +1140,78 @@
         <x:v>100</x:v>
       </x:c>
       <x:c r="B42" s="9" t="s">
-        <x:v>10</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="C42" s="9" t="s">
-        <x:v>51</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="D42" s="12" t="n">
-        <x:v>45888</x:v>
+        <x:v>45847</x:v>
       </x:c>
       <x:c r="E42" s="9" t="s">
-        <x:v>101</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="F42"/>
     </x:row>
     <x:row r="43" ht="13.05" customHeight="1">
       <x:c r="A43" s="9" t="s">
-        <x:v>102</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="B43" s="9" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="C43" s="9" t="s">
-        <x:v>34</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="D43" s="12" t="n">
-        <x:v>45848</x:v>
+        <x:v>45888</x:v>
       </x:c>
       <x:c r="E43" s="9" t="s">
-        <x:v>103</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="F43"/>
     </x:row>
     <x:row r="44" ht="13.05" customHeight="1">
       <x:c r="A44" s="9" t="s">
-        <x:v>104</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="B44" s="9" t="s">
-        <x:v>105</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="C44" s="9" t="s">
-        <x:v>51</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="D44" s="12" t="n">
-        <x:v>45895</x:v>
+        <x:v>45848</x:v>
       </x:c>
       <x:c r="E44" s="9" t="s">
         <x:v>106</x:v>
       </x:c>
       <x:c r="F44"/>
+    </x:row>
+    <x:row r="45" ht="13.05" customHeight="1">
+      <x:c r="A45" s="9" t="s">
+        <x:v>107</x:v>
+      </x:c>
+      <x:c r="B45" s="9" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="C45" s="9" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="D45" s="12" t="n">
+        <x:v>45895</x:v>
+      </x:c>
+      <x:c r="E45" s="9" t="s">
+        <x:v>108</x:v>
+      </x:c>
+      <x:c r="F45"/>
     </x:row>
   </x:sheetData>
   <x:pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
   <x:pageSetup paperSize="1" fitToWidth="1" fitToHeight="1" orientation="portrait"/>
+  <x:rowBreaks count="1" manualBreakCount="1">
+    <x:brk id="45" min="1" max="6" man="1"/>
+  </x:rowBreaks>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
One-click update from Van Paper 09:03 AM on 2025-09-22
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -52,6 +52,18 @@
     <x:t>0008143</x:t>
   </x:si>
   <x:si>
+    <x:t>ESCAPE CLEANING COMPANY LLC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Zigan, Gerald L</x:t>
+  </x:si>
+  <x:si>
+    <x:t>030</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008145</x:t>
+  </x:si>
+  <x:si>
     <x:t>ROYAL GOLF CLUB</x:t>
   </x:si>
   <x:si>
@@ -166,9 +178,6 @@
     <x:t>BARISTA COFFEE BAR</x:t>
   </x:si>
   <x:si>
-    <x:t>030</x:t>
-  </x:si>
-  <x:si>
     <x:t>0008227</x:t>
   </x:si>
   <x:si>
@@ -305,9 +314,6 @@
   </x:si>
   <x:si>
     <x:t>Fiesta Mexicana</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Zigan, Gerald L</x:t>
   </x:si>
   <x:si>
     <x:t>0008306</x:t>
@@ -423,7 +429,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:F45"/>
+  <x:dimension ref="A1:F46"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -499,148 +505,148 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="C4" s="9" t="s">
-        <x:v>7</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="D4" s="12" t="n">
-        <x:v>45868</x:v>
+        <x:v>45919</x:v>
       </x:c>
       <x:c r="E4" s="9" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="F4"/>
     </x:row>
     <x:row r="5" ht="13.05" customHeight="1">
       <x:c r="A5" s="9" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="B5" s="9" t="s">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="C5" s="9" t="s">
         <x:v>7</x:v>
       </x:c>
       <x:c r="D5" s="12" t="n">
-        <x:v>45883</x:v>
+        <x:v>45868</x:v>
       </x:c>
       <x:c r="E5" s="9" t="s">
-        <x:v>18</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="F5"/>
     </x:row>
     <x:row r="6" ht="13.05" customHeight="1">
       <x:c r="A6" s="9" t="s">
-        <x:v>19</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="B6" s="9" t="s">
-        <x:v>17</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C6" s="9" t="s">
         <x:v>7</x:v>
       </x:c>
       <x:c r="D6" s="12" t="n">
-        <x:v>45884</x:v>
+        <x:v>45883</x:v>
       </x:c>
       <x:c r="E6" s="9" t="s">
-        <x:v>20</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F6"/>
     </x:row>
     <x:row r="7" ht="13.05" customHeight="1">
       <x:c r="A7" s="9" t="s">
-        <x:v>16</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="B7" s="9" t="s">
-        <x:v>17</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C7" s="9" t="s">
         <x:v>7</x:v>
       </x:c>
       <x:c r="D7" s="12" t="n">
-        <x:v>45883</x:v>
+        <x:v>45884</x:v>
       </x:c>
       <x:c r="E7" s="9" t="s">
-        <x:v>21</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="F7"/>
     </x:row>
     <x:row r="8" ht="13.05" customHeight="1">
       <x:c r="A8" s="9" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="B8" s="9" t="s">
-        <x:v>17</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C8" s="9" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="D8" s="13"/>
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D8" s="12" t="n">
+        <x:v>45883</x:v>
+      </x:c>
       <x:c r="E8" s="9" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="F8"/>
     </x:row>
     <x:row r="9" ht="13.05" customHeight="1">
       <x:c r="A9" s="9" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B9" s="9" t="s">
-        <x:v>17</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C9" s="9" t="s">
-        <x:v>23</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="D9" s="13"/>
       <x:c r="E9" s="9" t="s">
-        <x:v>26</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="F9"/>
     </x:row>
     <x:row r="10" ht="13.05" customHeight="1">
       <x:c r="A10" s="9" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="B10" s="9" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C10" s="9" t="s">
         <x:v>27</x:v>
-      </x:c>
-      <x:c r="B10" s="9" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="C10" s="9" t="s">
-        <x:v>7</x:v>
       </x:c>
       <x:c r="D10" s="13"/>
       <x:c r="E10" s="9" t="s">
-        <x:v>28</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="F10"/>
     </x:row>
     <x:row r="11" ht="13.05" customHeight="1">
       <x:c r="A11" s="9" t="s">
-        <x:v>29</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="B11" s="9" t="s">
-        <x:v>30</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C11" s="9" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="D11" s="12" t="n">
-        <x:v>45874</x:v>
-      </x:c>
+      <x:c r="D11" s="13"/>
       <x:c r="E11" s="9" t="s">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="F11"/>
     </x:row>
     <x:row r="12" ht="13.05" customHeight="1">
       <x:c r="A12" s="9" t="s">
-        <x:v>32</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="B12" s="9" t="s">
-        <x:v>33</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="C12" s="9" t="s">
-        <x:v>34</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D12" s="12" t="n">
-        <x:v>45849</x:v>
+        <x:v>45874</x:v>
       </x:c>
       <x:c r="E12" s="9" t="s">
         <x:v>35</x:v>
@@ -652,182 +658,182 @@
         <x:v>36</x:v>
       </x:c>
       <x:c r="B13" s="9" t="s">
-        <x:v>33</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="C13" s="9" t="s">
-        <x:v>34</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="D13" s="12" t="n">
-        <x:v>45845</x:v>
+        <x:v>45849</x:v>
       </x:c>
       <x:c r="E13" s="9" t="s">
-        <x:v>37</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="F13"/>
     </x:row>
     <x:row r="14" ht="13.05" customHeight="1">
       <x:c r="A14" s="9" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="B14" s="9" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="C14" s="9" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="B14" s="9" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="C14" s="9" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D14" s="13"/>
+      <x:c r="D14" s="12" t="n">
+        <x:v>45845</x:v>
+      </x:c>
       <x:c r="E14" s="9" t="s">
-        <x:v>39</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="F14"/>
     </x:row>
     <x:row r="15" ht="13.05" customHeight="1">
       <x:c r="A15" s="9" t="s">
-        <x:v>40</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="B15" s="9" t="s">
-        <x:v>41</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C15" s="9" t="s">
-        <x:v>11</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D15" s="13"/>
       <x:c r="E15" s="9" t="s">
-        <x:v>42</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="F15"/>
     </x:row>
     <x:row r="16" ht="13.05" customHeight="1">
       <x:c r="A16" s="9" t="s">
-        <x:v>43</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="B16" s="9" t="s">
-        <x:v>44</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="C16" s="9" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D16" s="12" t="n">
-        <x:v>45855</x:v>
-      </x:c>
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D16" s="13"/>
       <x:c r="E16" s="9" t="s">
-        <x:v>45</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="F16"/>
     </x:row>
     <x:row r="17" ht="13.05" customHeight="1">
       <x:c r="A17" s="9" t="s">
-        <x:v>46</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="B17" s="9" t="s">
-        <x:v>17</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="C17" s="9" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="D17" s="13"/>
+      <x:c r="D17" s="12" t="n">
+        <x:v>45855</x:v>
+      </x:c>
       <x:c r="E17" s="9" t="s">
-        <x:v>47</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="F17"/>
     </x:row>
     <x:row r="18" ht="13.05" customHeight="1">
       <x:c r="A18" s="9" t="s">
-        <x:v>48</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="B18" s="9" t="s">
-        <x:v>33</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C18" s="9" t="s">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="D18" s="12" t="n">
-        <x:v>45873</x:v>
-      </x:c>
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D18" s="13"/>
       <x:c r="E18" s="9" t="s">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="F18"/>
     </x:row>
     <x:row r="19" ht="13.05" customHeight="1">
       <x:c r="A19" s="9" t="s">
-        <x:v>50</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="B19" s="9" t="s">
-        <x:v>10</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="C19" s="9" t="s">
-        <x:v>51</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="D19" s="12" t="n">
-        <x:v>45883</x:v>
+        <x:v>45873</x:v>
       </x:c>
       <x:c r="E19" s="9" t="s">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="F19"/>
     </x:row>
     <x:row r="20" ht="13.05" customHeight="1">
       <x:c r="A20" s="9" t="s">
-        <x:v>53</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="B20" s="9" t="s">
-        <x:v>41</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="C20" s="9" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="D20" s="13"/>
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="D20" s="12" t="n">
+        <x:v>45883</x:v>
+      </x:c>
       <x:c r="E20" s="9" t="s">
-        <x:v>54</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="F20"/>
     </x:row>
     <x:row r="21" ht="13.05" customHeight="1">
       <x:c r="A21" s="9" t="s">
-        <x:v>55</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="B21" s="9" t="s">
-        <x:v>17</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="C21" s="9" t="s">
-        <x:v>7</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="D21" s="13"/>
       <x:c r="E21" s="9" t="s">
-        <x:v>56</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="F21"/>
     </x:row>
     <x:row r="22" ht="13.05" customHeight="1">
       <x:c r="A22" s="9" t="s">
-        <x:v>57</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="B22" s="9" t="s">
-        <x:v>14</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C22" s="9" t="s">
-        <x:v>23</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D22" s="13"/>
       <x:c r="E22" s="9" t="s">
-        <x:v>58</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="F22"/>
     </x:row>
     <x:row r="23" ht="13.05" customHeight="1">
       <x:c r="A23" s="9" t="s">
-        <x:v>59</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="B23" s="9" t="s">
-        <x:v>60</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="C23" s="9" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="D23" s="12" t="n">
-        <x:v>45881</x:v>
-      </x:c>
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="D23" s="13"/>
       <x:c r="E23" s="9" t="s">
         <x:v>61</x:v>
       </x:c>
@@ -838,48 +844,50 @@
         <x:v>62</x:v>
       </x:c>
       <x:c r="B24" s="9" t="s">
-        <x:v>41</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="C24" s="9" t="s">
-        <x:v>51</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="D24" s="12" t="n">
-        <x:v>45883</x:v>
+        <x:v>45881</x:v>
       </x:c>
       <x:c r="E24" s="9" t="s">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="F24"/>
     </x:row>
     <x:row r="25" ht="13.05" customHeight="1">
       <x:c r="A25" s="9" t="s">
-        <x:v>64</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="B25" s="9" t="s">
-        <x:v>33</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="C25" s="9" t="s">
-        <x:v>34</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="D25" s="12" t="n">
-        <x:v>45911</x:v>
+        <x:v>45883</x:v>
       </x:c>
       <x:c r="E25" s="9" t="s">
-        <x:v>65</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="F25"/>
     </x:row>
     <x:row r="26" ht="13.05" customHeight="1">
       <x:c r="A26" s="9" t="s">
-        <x:v>66</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="B26" s="9" t="s">
-        <x:v>67</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="C26" s="9" t="s">
-        <x:v>51</x:v>
-      </x:c>
-      <x:c r="D26" s="13"/>
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="D26" s="12" t="n">
+        <x:v>45911</x:v>
+      </x:c>
       <x:c r="E26" s="9" t="s">
         <x:v>68</x:v>
       </x:c>
@@ -890,244 +898,244 @@
         <x:v>69</x:v>
       </x:c>
       <x:c r="B27" s="9" t="s">
-        <x:v>33</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="C27" s="9" t="s">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="D27" s="12" t="n">
-        <x:v>45895</x:v>
-      </x:c>
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="D27" s="13"/>
       <x:c r="E27" s="9" t="s">
-        <x:v>70</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="F27"/>
     </x:row>
     <x:row r="28" ht="13.05" customHeight="1">
       <x:c r="A28" s="9" t="s">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="B28" s="9" t="s">
-        <x:v>33</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="C28" s="9" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="D28" s="13"/>
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="D28" s="12" t="n">
+        <x:v>45895</x:v>
+      </x:c>
       <x:c r="E28" s="9" t="s">
-        <x:v>72</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="F28"/>
     </x:row>
     <x:row r="29" ht="13.05" customHeight="1">
       <x:c r="A29" s="9" t="s">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="B29" s="9" t="s">
-        <x:v>17</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="C29" s="9" t="s">
-        <x:v>7</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="D29" s="13"/>
       <x:c r="E29" s="9" t="s">
-        <x:v>74</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="F29"/>
     </x:row>
     <x:row r="30" ht="13.05" customHeight="1">
       <x:c r="A30" s="9" t="s">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="B30" s="9" t="s">
-        <x:v>17</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C30" s="9" t="s">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="D30" s="12" t="n">
-        <x:v>45910</x:v>
-      </x:c>
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D30" s="13"/>
       <x:c r="E30" s="9" t="s">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="F30"/>
     </x:row>
     <x:row r="31" ht="13.05" customHeight="1">
       <x:c r="A31" s="9" t="s">
-        <x:v>77</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="B31" s="9" t="s">
-        <x:v>17</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C31" s="9" t="s">
-        <x:v>7</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="D31" s="12" t="n">
-        <x:v>45911</x:v>
+        <x:v>45910</x:v>
       </x:c>
       <x:c r="E31" s="9" t="s">
-        <x:v>78</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="F31"/>
     </x:row>
     <x:row r="32" ht="13.05" customHeight="1">
       <x:c r="A32" s="9" t="s">
-        <x:v>79</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="B32" s="9" t="s">
-        <x:v>17</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C32" s="9" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="D32" s="13"/>
+      <x:c r="D32" s="12" t="n">
+        <x:v>45911</x:v>
+      </x:c>
       <x:c r="E32" s="9" t="s">
-        <x:v>80</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="F32"/>
     </x:row>
     <x:row r="33" ht="13.05" customHeight="1">
       <x:c r="A33" s="9" t="s">
-        <x:v>81</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="B33" s="9" t="s">
-        <x:v>33</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C33" s="9" t="s">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="D33" s="12" t="n">
-        <x:v>45896</x:v>
-      </x:c>
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D33" s="13"/>
       <x:c r="E33" s="9" t="s">
-        <x:v>82</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="F33"/>
     </x:row>
     <x:row r="34" ht="13.05" customHeight="1">
       <x:c r="A34" s="9" t="s">
-        <x:v>83</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="B34" s="9" t="s">
-        <x:v>14</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="C34" s="9" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="D34" s="13"/>
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="D34" s="12" t="n">
+        <x:v>45896</x:v>
+      </x:c>
       <x:c r="E34" s="9" t="s">
-        <x:v>84</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="F34"/>
     </x:row>
     <x:row r="35" ht="13.05" customHeight="1">
       <x:c r="A35" s="9" t="s">
-        <x:v>85</x:v>
-      </x:c>
-      <x:c r="B35" s="13"/>
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="B35" s="9" t="s">
+        <x:v>18</x:v>
+      </x:c>
       <x:c r="C35" s="9" t="s">
-        <x:v>11</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="D35" s="13"/>
       <x:c r="E35" s="9" t="s">
-        <x:v>86</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="F35"/>
     </x:row>
     <x:row r="36" ht="13.05" customHeight="1">
       <x:c r="A36" s="9" t="s">
-        <x:v>87</x:v>
-      </x:c>
-      <x:c r="B36" s="9" t="s">
-        <x:v>14</x:v>
-      </x:c>
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="B36" s="13"/>
       <x:c r="C36" s="9" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="D36" s="12" t="n">
-        <x:v>45912</x:v>
-      </x:c>
+      <x:c r="D36" s="13"/>
       <x:c r="E36" s="9" t="s">
-        <x:v>88</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="F36"/>
     </x:row>
     <x:row r="37" ht="13.05" customHeight="1">
       <x:c r="A37" s="9" t="s">
-        <x:v>89</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="B37" s="9" t="s">
-        <x:v>33</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="C37" s="9" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="D37" s="13"/>
+      <x:c r="D37" s="12" t="n">
+        <x:v>45912</x:v>
+      </x:c>
       <x:c r="E37" s="9" t="s">
-        <x:v>90</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="F37"/>
     </x:row>
     <x:row r="38" ht="13.05" customHeight="1">
       <x:c r="A38" s="9" t="s">
-        <x:v>91</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="B38" s="9" t="s">
-        <x:v>17</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="C38" s="9" t="s">
-        <x:v>7</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="D38" s="13"/>
       <x:c r="E38" s="9" t="s">
-        <x:v>92</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="F38"/>
     </x:row>
     <x:row r="39" ht="13.05" customHeight="1">
       <x:c r="A39" s="9" t="s">
-        <x:v>93</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="B39" s="9" t="s">
-        <x:v>33</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C39" s="9" t="s">
-        <x:v>51</x:v>
-      </x:c>
-      <x:c r="D39" s="12" t="n">
-        <x:v>45916</x:v>
-      </x:c>
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D39" s="13"/>
       <x:c r="E39" s="9" t="s">
-        <x:v>94</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="F39"/>
     </x:row>
     <x:row r="40" ht="13.05" customHeight="1">
       <x:c r="A40" s="9" t="s">
-        <x:v>95</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="B40" s="9" t="s">
-        <x:v>41</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="C40" s="9" t="s">
-        <x:v>51</x:v>
-      </x:c>
-      <x:c r="D40" s="13"/>
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="D40" s="12" t="n">
+        <x:v>45916</x:v>
+      </x:c>
       <x:c r="E40" s="9" t="s">
-        <x:v>96</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="F40"/>
     </x:row>
     <x:row r="41" ht="13.05" customHeight="1">
       <x:c r="A41" s="9" t="s">
-        <x:v>97</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="B41" s="9" t="s">
-        <x:v>98</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="C41" s="9" t="s">
-        <x:v>51</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="D41" s="13"/>
       <x:c r="E41" s="9" t="s">
@@ -1140,31 +1148,29 @@
         <x:v>100</x:v>
       </x:c>
       <x:c r="B42" s="9" t="s">
-        <x:v>30</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="C42" s="9" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="D42" s="13"/>
+      <x:c r="E42" s="9" t="s">
         <x:v>101</x:v>
-      </x:c>
-      <x:c r="D42" s="12" t="n">
-        <x:v>45847</x:v>
-      </x:c>
-      <x:c r="E42" s="9" t="s">
-        <x:v>102</x:v>
       </x:c>
       <x:c r="F42"/>
     </x:row>
     <x:row r="43" ht="13.05" customHeight="1">
       <x:c r="A43" s="9" t="s">
+        <x:v>102</x:v>
+      </x:c>
+      <x:c r="B43" s="9" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="C43" s="9" t="s">
         <x:v>103</x:v>
       </x:c>
-      <x:c r="B43" s="9" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C43" s="9" t="s">
-        <x:v>51</x:v>
-      </x:c>
       <x:c r="D43" s="12" t="n">
-        <x:v>45888</x:v>
+        <x:v>45847</x:v>
       </x:c>
       <x:c r="E43" s="9" t="s">
         <x:v>104</x:v>
@@ -1179,10 +1185,10 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="C44" s="9" t="s">
-        <x:v>34</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="D44" s="12" t="n">
-        <x:v>45848</x:v>
+        <x:v>45888</x:v>
       </x:c>
       <x:c r="E44" s="9" t="s">
         <x:v>106</x:v>
@@ -1194,24 +1200,42 @@
         <x:v>107</x:v>
       </x:c>
       <x:c r="B45" s="9" t="s">
-        <x:v>98</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="C45" s="9" t="s">
-        <x:v>51</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="D45" s="12" t="n">
-        <x:v>45895</x:v>
+        <x:v>45848</x:v>
       </x:c>
       <x:c r="E45" s="9" t="s">
         <x:v>108</x:v>
       </x:c>
       <x:c r="F45"/>
+    </x:row>
+    <x:row r="46" ht="13.05" customHeight="1">
+      <x:c r="A46" s="9" t="s">
+        <x:v>109</x:v>
+      </x:c>
+      <x:c r="B46" s="9" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="C46" s="9" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="D46" s="12" t="n">
+        <x:v>45895</x:v>
+      </x:c>
+      <x:c r="E46" s="9" t="s">
+        <x:v>110</x:v>
+      </x:c>
+      <x:c r="F46"/>
     </x:row>
   </x:sheetData>
   <x:pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
   <x:pageSetup paperSize="1" fitToWidth="1" fitToHeight="1" orientation="portrait"/>
   <x:rowBreaks count="1" manualBreakCount="1">
-    <x:brk id="45" min="1" max="6" man="1"/>
+    <x:brk id="46" min="1" max="6" man="1"/>
   </x:rowBreaks>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
One-click update from Van Paper 08:02 AM on 2025-10-02
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -116,6 +116,27 @@
   </x:si>
   <x:si>
     <x:t>0008324</x:t>
+  </x:si>
+  <x:si>
+    <x:t>YOUNG'S</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Larsen, Rick J</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008325</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MARMA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008326</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BLOSSOM BRIDGE CHILD CARE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008327</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -201,7 +222,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:F10"/>
+  <x:dimension ref="A1:F13"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -383,6 +404,54 @@
       </x:c>
       <x:c r="F10"/>
     </x:row>
+    <x:row r="11" ht="13.05" customHeight="1">
+      <x:c r="A11" s="9" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="B11" s="9" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="C11" s="9" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="D11" s="13"/>
+      <x:c r="E11" s="9" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="F11"/>
+    </x:row>
+    <x:row r="12" ht="13.05" customHeight="1">
+      <x:c r="A12" s="9" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="B12" s="9" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="C12" s="9" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="D12" s="13"/>
+      <x:c r="E12" s="9" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="F12"/>
+    </x:row>
+    <x:row r="13" ht="13.05" customHeight="1">
+      <x:c r="A13" s="9" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="B13" s="9" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="C13" s="9" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="D13" s="13"/>
+      <x:c r="E13" s="9" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="F13"/>
+    </x:row>
   </x:sheetData>
   <x:pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
   <x:pageSetup paperSize="1" fitToWidth="1" fitToHeight="1" orientation="portrait"/>

</xml_diff>

<commit_message>
One-click update from Van Paper 07:43 AM on 2025-10-06
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -137,6 +137,27 @@
   </x:si>
   <x:si>
     <x:t>0008327</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Paradise Smoothie Cafe </x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008329</x:t>
+  </x:si>
+  <x:si>
+    <x:t>OWEN MEATS CORP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008331</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HOLY FAMILY MARONITE CHURCH</x:t>
+  </x:si>
+  <x:si>
+    <x:t>003</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0004965</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -222,7 +243,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:F13"/>
+  <x:dimension ref="A1:F16"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -452,6 +473,56 @@
       </x:c>
       <x:c r="F13"/>
     </x:row>
+    <x:row r="14" ht="13.05" customHeight="1">
+      <x:c r="A14" s="9" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="B14" s="9" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="C14" s="9" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="D14" s="13"/>
+      <x:c r="E14" s="9" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="F14"/>
+    </x:row>
+    <x:row r="15" ht="13.05" customHeight="1">
+      <x:c r="A15" s="9" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="B15" s="9" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C15" s="9" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D15" s="13"/>
+      <x:c r="E15" s="9" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="F15"/>
+    </x:row>
+    <x:row r="16" ht="13.05" customHeight="1">
+      <x:c r="A16" s="9" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="B16" s="9" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="C16" s="9" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="D16" s="12" t="n">
+        <x:v>45932</x:v>
+      </x:c>
+      <x:c r="E16" s="9" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="F16"/>
+    </x:row>
   </x:sheetData>
   <x:pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
   <x:pageSetup paperSize="1" fitToWidth="1" fitToHeight="1" orientation="portrait"/>

</xml_diff>

<commit_message>
One-click update from Van Paper 08:06 AM on 2025-10-09
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -149,6 +149,12 @@
   </x:si>
   <x:si>
     <x:t>0008331</x:t>
+  </x:si>
+  <x:si>
+    <x:t>VINCENT MANUFACTURING</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008335</x:t>
   </x:si>
   <x:si>
     <x:t>HOLY FAMILY MARONITE CHURCH</x:t>
@@ -243,7 +249,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:F16"/>
+  <x:dimension ref="A1:F17"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -510,18 +516,34 @@
         <x:v>46</x:v>
       </x:c>
       <x:c r="B16" s="9" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="C16" s="9" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D16" s="13"/>
+      <x:c r="E16" s="9" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="F16"/>
+    </x:row>
+    <x:row r="17" ht="13.05" customHeight="1">
+      <x:c r="A17" s="9" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="B17" s="9" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="C16" s="9" t="s">
-        <x:v>47</x:v>
-      </x:c>
-      <x:c r="D16" s="12" t="n">
+      <x:c r="C17" s="9" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="D17" s="12" t="n">
         <x:v>45932</x:v>
       </x:c>
-      <x:c r="E16" s="9" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="F16"/>
+      <x:c r="E17" s="9" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="F17"/>
     </x:row>
   </x:sheetData>
   <x:pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
One-click update from Van Paper 07:09 AM on 2025-10-10
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -505,7 +505,9 @@
       <x:c r="C15" s="9" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="D15" s="13"/>
+      <x:c r="D15" s="12" t="n">
+        <x:v>45939</x:v>
+      </x:c>
       <x:c r="E15" s="9" t="s">
         <x:v>45</x:v>
       </x:c>

</xml_diff>

<commit_message>
One-click update from Van Paper 07:22 AM on 2025-10-14
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -155,6 +155,12 @@
   </x:si>
   <x:si>
     <x:t>0008335</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BEHRMAV ENTERPRISES LLC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008337</x:t>
   </x:si>
   <x:si>
     <x:t>HOLY FAMILY MARONITE CHURCH</x:t>
@@ -249,7 +255,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:F17"/>
+  <x:dimension ref="A1:F18"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -534,18 +540,34 @@
         <x:v>48</x:v>
       </x:c>
       <x:c r="B17" s="9" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="C17" s="9" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="D17" s="13"/>
+      <x:c r="E17" s="9" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="F17"/>
+    </x:row>
+    <x:row r="18" ht="13.05" customHeight="1">
+      <x:c r="A18" s="9" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="B18" s="9" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="C17" s="9" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="D17" s="12" t="n">
+      <x:c r="C18" s="9" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="D18" s="12" t="n">
         <x:v>45932</x:v>
       </x:c>
-      <x:c r="E17" s="9" t="s">
-        <x:v>50</x:v>
-      </x:c>
-      <x:c r="F17"/>
+      <x:c r="E18" s="9" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="F18"/>
     </x:row>
   </x:sheetData>
   <x:pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
One-click update from Van Paper 07:06 AM on 2025-10-15
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -161,6 +161,18 @@
   </x:si>
   <x:si>
     <x:t>0008337</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DUMPLING EATERY</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008338</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HEARTH LLC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008339</x:t>
   </x:si>
   <x:si>
     <x:t>HOLY FAMILY MARONITE CHURCH</x:t>
@@ -255,7 +267,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:F18"/>
+  <x:dimension ref="A1:F20"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -556,18 +568,50 @@
         <x:v>50</x:v>
       </x:c>
       <x:c r="B18" s="9" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C18" s="9" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D18" s="13"/>
+      <x:c r="E18" s="9" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="F18"/>
+    </x:row>
+    <x:row r="19" ht="13.05" customHeight="1">
+      <x:c r="A19" s="9" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="B19" s="9" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C19" s="9" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="D19" s="13"/>
+      <x:c r="E19" s="9" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="F19"/>
+    </x:row>
+    <x:row r="20" ht="13.05" customHeight="1">
+      <x:c r="A20" s="9" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="B20" s="9" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="C18" s="9" t="s">
-        <x:v>51</x:v>
-      </x:c>
-      <x:c r="D18" s="12" t="n">
+      <x:c r="C20" s="9" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="D20" s="12" t="n">
         <x:v>45932</x:v>
       </x:c>
-      <x:c r="E18" s="9" t="s">
-        <x:v>52</x:v>
-      </x:c>
-      <x:c r="F18"/>
+      <x:c r="E20" s="9" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="F20"/>
     </x:row>
   </x:sheetData>
   <x:pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
One-click update from Van Paper 07:06 AM on 2025-10-17
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -573,7 +573,9 @@
       <x:c r="C18" s="9" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="D18" s="13"/>
+      <x:c r="D18" s="12" t="n">
+        <x:v>45946</x:v>
+      </x:c>
       <x:c r="E18" s="9" t="s">
         <x:v>51</x:v>
       </x:c>

</xml_diff>

<commit_message>
One-click update from Van Paper 07:22 AM on 2025-10-21
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -163,7 +163,7 @@
     <x:t>0008337</x:t>
   </x:si>
   <x:si>
-    <x:t>DUMPLING EATERY</x:t>
+    <x:t>DUMPLING HOUSE EP</x:t>
   </x:si>
   <x:si>
     <x:t>0008338</x:t>
@@ -173,6 +173,21 @@
   </x:si>
   <x:si>
     <x:t>0008339</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ELITE LIQUOR INC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008344</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Executive Aviation</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Dack, Suzanne</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008345</x:t>
   </x:si>
   <x:si>
     <x:t>HOLY FAMILY MARONITE CHURCH</x:t>
@@ -267,7 +282,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:F20"/>
+  <x:dimension ref="A1:F22"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -427,7 +442,9 @@
       <x:c r="C9" s="9" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="D9" s="13"/>
+      <x:c r="D9" s="12" t="n">
+        <x:v>45950</x:v>
+      </x:c>
       <x:c r="E9" s="9" t="s">
         <x:v>31</x:v>
       </x:c>
@@ -602,18 +619,50 @@
         <x:v>54</x:v>
       </x:c>
       <x:c r="B20" s="9" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="C20" s="9" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="D20" s="13"/>
+      <x:c r="E20" s="9" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="F20"/>
+    </x:row>
+    <x:row r="21" ht="13.05" customHeight="1">
+      <x:c r="A21" s="9" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="B21" s="9" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="C21" s="9" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="D21" s="13"/>
+      <x:c r="E21" s="9" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="F21"/>
+    </x:row>
+    <x:row r="22" ht="13.05" customHeight="1">
+      <x:c r="A22" s="9" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="B22" s="9" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="C20" s="9" t="s">
-        <x:v>55</x:v>
-      </x:c>
-      <x:c r="D20" s="12" t="n">
+      <x:c r="C22" s="9" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="D22" s="12" t="n">
         <x:v>45932</x:v>
       </x:c>
-      <x:c r="E20" s="9" t="s">
-        <x:v>56</x:v>
-      </x:c>
-      <x:c r="F20"/>
+      <x:c r="E22" s="9" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="F22"/>
     </x:row>
   </x:sheetData>
   <x:pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
One-click update from Van Paper 07:26 AM on 2025-10-23
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -188,6 +188,12 @@
   </x:si>
   <x:si>
     <x:t>0008345</x:t>
+  </x:si>
+  <x:si>
+    <x:t>WOODBURY ICE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008347</x:t>
   </x:si>
   <x:si>
     <x:t>HOLY FAMILY MARONITE CHURCH</x:t>
@@ -282,7 +288,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:F22"/>
+  <x:dimension ref="A1:F23"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -651,18 +657,34 @@
         <x:v>59</x:v>
       </x:c>
       <x:c r="B22" s="9" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C22" s="9" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="D22" s="13"/>
+      <x:c r="E22" s="9" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="F22"/>
+    </x:row>
+    <x:row r="23" ht="13.05" customHeight="1">
+      <x:c r="A23" s="9" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="B23" s="9" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="C22" s="9" t="s">
-        <x:v>60</x:v>
-      </x:c>
-      <x:c r="D22" s="12" t="n">
+      <x:c r="C23" s="9" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="D23" s="12" t="n">
         <x:v>45932</x:v>
       </x:c>
-      <x:c r="E22" s="9" t="s">
-        <x:v>61</x:v>
-      </x:c>
-      <x:c r="F22"/>
+      <x:c r="E23" s="9" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="F23"/>
     </x:row>
   </x:sheetData>
   <x:pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
One-click update from Van Paper 07:11 AM on 2025-10-27
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -196,6 +196,15 @@
     <x:t>0008347</x:t>
   </x:si>
   <x:si>
+    <x:t>ROSALIA LLC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cina, Jonathan D</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008350</x:t>
+  </x:si>
+  <x:si>
     <x:t>HOLY FAMILY MARONITE CHURCH</x:t>
   </x:si>
   <x:si>
@@ -203,6 +212,15 @@
   </x:si>
   <x:si>
     <x:t>0004965</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SCHMITT MUSIC CTR</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Monroe, Michael D</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0005169</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -288,7 +306,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:F23"/>
+  <x:dimension ref="A1:F25"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -630,7 +648,9 @@
       <x:c r="C20" s="9" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="D20" s="13"/>
+      <x:c r="D20" s="12" t="n">
+        <x:v>45954</x:v>
+      </x:c>
       <x:c r="E20" s="9" t="s">
         <x:v>55</x:v>
       </x:c>
@@ -673,18 +693,52 @@
         <x:v>61</x:v>
       </x:c>
       <x:c r="B23" s="9" t="s">
-        <x:v>26</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="C23" s="9" t="s">
-        <x:v>62</x:v>
-      </x:c>
-      <x:c r="D23" s="12" t="n">
-        <x:v>45932</x:v>
-      </x:c>
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="D23" s="13"/>
       <x:c r="E23" s="9" t="s">
         <x:v>63</x:v>
       </x:c>
       <x:c r="F23"/>
+    </x:row>
+    <x:row r="24" ht="13.05" customHeight="1">
+      <x:c r="A24" s="9" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="B24" s="9" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="C24" s="9" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="D24" s="12" t="n">
+        <x:v>45932</x:v>
+      </x:c>
+      <x:c r="E24" s="9" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="F24"/>
+    </x:row>
+    <x:row r="25" ht="13.05" customHeight="1">
+      <x:c r="A25" s="9" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="B25" s="9" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="C25" s="9" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="D25" s="12" t="n">
+        <x:v>45954</x:v>
+      </x:c>
+      <x:c r="E25" s="9" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="F25"/>
     </x:row>
   </x:sheetData>
   <x:pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
One-click update from Van Paper 07:06 AM on 2025-10-29
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -203,6 +203,12 @@
   </x:si>
   <x:si>
     <x:t>0008350</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MSP COMMERCIAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008352</x:t>
   </x:si>
   <x:si>
     <x:t>HOLY FAMILY MARONITE CHURCH</x:t>
@@ -306,7 +312,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:F25"/>
+  <x:dimension ref="A1:F26"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -630,7 +636,7 @@
         <x:v>33</x:v>
       </x:c>
       <x:c r="C19" s="9" t="s">
-        <x:v>15</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="D19" s="13"/>
       <x:c r="E19" s="9" t="s">
@@ -709,36 +715,52 @@
         <x:v>64</x:v>
       </x:c>
       <x:c r="B24" s="9" t="s">
-        <x:v>26</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="C24" s="9" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="D24" s="13"/>
+      <x:c r="E24" s="9" t="s">
         <x:v>65</x:v>
-      </x:c>
-      <x:c r="D24" s="12" t="n">
-        <x:v>45932</x:v>
-      </x:c>
-      <x:c r="E24" s="9" t="s">
-        <x:v>66</x:v>
       </x:c>
       <x:c r="F24"/>
     </x:row>
     <x:row r="25" ht="13.05" customHeight="1">
       <x:c r="A25" s="9" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="B25" s="9" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="C25" s="9" t="s">
         <x:v>67</x:v>
       </x:c>
-      <x:c r="B25" s="9" t="s">
+      <x:c r="D25" s="12" t="n">
+        <x:v>45932</x:v>
+      </x:c>
+      <x:c r="E25" s="9" t="s">
         <x:v>68</x:v>
       </x:c>
-      <x:c r="C25" s="9" t="s">
-        <x:v>65</x:v>
-      </x:c>
-      <x:c r="D25" s="12" t="n">
+      <x:c r="F25"/>
+    </x:row>
+    <x:row r="26" ht="13.05" customHeight="1">
+      <x:c r="A26" s="9" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="B26" s="9" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="C26" s="9" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="D26" s="12" t="n">
         <x:v>45954</x:v>
       </x:c>
-      <x:c r="E25" s="9" t="s">
-        <x:v>69</x:v>
-      </x:c>
-      <x:c r="F25"/>
+      <x:c r="E26" s="9" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="F26"/>
     </x:row>
   </x:sheetData>
   <x:pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
One-click update from Van Paper 07:22 AM on 2025-10-30
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -52,7 +52,7 @@
     <x:t>0008209</x:t>
   </x:si>
   <x:si>
-    <x:t>DREAMSTATE CAFE</x:t>
+    <x:t>BOMBUS CONCEPTS LLC</x:t>
   </x:si>
   <x:si>
     <x:t>McGivern, Kelly W</x:t>
@@ -638,7 +638,9 @@
       <x:c r="C19" s="9" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="D19" s="13"/>
+      <x:c r="D19" s="12" t="n">
+        <x:v>45959</x:v>
+      </x:c>
       <x:c r="E19" s="9" t="s">
         <x:v>53</x:v>
       </x:c>

</xml_diff>

<commit_message>
One-click update from Van Paper 07:10 AM on 2025-10-31
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -52,6 +52,15 @@
     <x:t>0008209</x:t>
   </x:si>
   <x:si>
+    <x:t>LITTLE BIRD DELICATESSEN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cina, Jonathan D</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008303</x:t>
+  </x:si>
+  <x:si>
     <x:t>BOMBUS CONCEPTS LLC</x:t>
   </x:si>
   <x:si>
@@ -197,9 +206,6 @@
   </x:si>
   <x:si>
     <x:t>ROSALIA LLC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Cina, Jonathan D</x:t>
   </x:si>
   <x:si>
     <x:t>0008350</x:t>
@@ -312,7 +318,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:F26"/>
+  <x:dimension ref="A1:F27"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -388,59 +394,59 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="C4" s="9" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D4" s="12" t="n">
+        <x:v>45960</x:v>
+      </x:c>
+      <x:c r="E4" s="9" t="s">
         <x:v>15</x:v>
-      </x:c>
-      <x:c r="D4" s="13"/>
-      <x:c r="E4" s="9" t="s">
-        <x:v>16</x:v>
       </x:c>
       <x:c r="F4"/>
     </x:row>
     <x:row r="5" ht="13.05" customHeight="1">
       <x:c r="A5" s="9" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="B5" s="9" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="B5" s="9" t="s">
+      <x:c r="C5" s="9" t="s">
         <x:v>18</x:v>
-      </x:c>
-      <x:c r="C5" s="9" t="s">
-        <x:v>19</x:v>
       </x:c>
       <x:c r="D5" s="13"/>
       <x:c r="E5" s="9" t="s">
-        <x:v>20</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="F5"/>
     </x:row>
     <x:row r="6" ht="13.05" customHeight="1">
       <x:c r="A6" s="9" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B6" s="9" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="B6" s="9" t="s">
+      <x:c r="C6" s="9" t="s">
         <x:v>22</x:v>
-      </x:c>
-      <x:c r="C6" s="9" t="s">
-        <x:v>23</x:v>
       </x:c>
       <x:c r="D6" s="13"/>
       <x:c r="E6" s="9" t="s">
-        <x:v>24</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="F6"/>
     </x:row>
     <x:row r="7" ht="13.05" customHeight="1">
       <x:c r="A7" s="9" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B7" s="9" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="B7" s="9" t="s">
+      <x:c r="C7" s="9" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="C7" s="9" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="D7" s="12" t="n">
-        <x:v>45929</x:v>
-      </x:c>
+      <x:c r="D7" s="13"/>
       <x:c r="E7" s="9" t="s">
         <x:v>27</x:v>
       </x:c>
@@ -451,46 +457,48 @@
         <x:v>28</x:v>
       </x:c>
       <x:c r="B8" s="9" t="s">
-        <x:v>18</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="C8" s="9" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="D8" s="13"/>
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="D8" s="12" t="n">
+        <x:v>45929</x:v>
+      </x:c>
       <x:c r="E8" s="9" t="s">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="F8"/>
     </x:row>
     <x:row r="9" ht="13.05" customHeight="1">
       <x:c r="A9" s="9" t="s">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="B9" s="9" t="s">
-        <x:v>22</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C9" s="9" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="D9" s="12" t="n">
-        <x:v>45950</x:v>
-      </x:c>
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D9" s="13"/>
       <x:c r="E9" s="9" t="s">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="F9"/>
     </x:row>
     <x:row r="10" ht="13.05" customHeight="1">
       <x:c r="A10" s="9" t="s">
-        <x:v>32</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="B10" s="9" t="s">
-        <x:v>33</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="C10" s="9" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="D10" s="13"/>
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="D10" s="12" t="n">
+        <x:v>45950</x:v>
+      </x:c>
       <x:c r="E10" s="9" t="s">
         <x:v>34</x:v>
       </x:c>
@@ -504,7 +512,7 @@
         <x:v>36</x:v>
       </x:c>
       <x:c r="C11" s="9" t="s">
-        <x:v>15</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D11" s="13"/>
       <x:c r="E11" s="9" t="s">
@@ -517,164 +525,164 @@
         <x:v>38</x:v>
       </x:c>
       <x:c r="B12" s="9" t="s">
-        <x:v>36</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="C12" s="9" t="s">
-        <x:v>15</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D12" s="13"/>
       <x:c r="E12" s="9" t="s">
-        <x:v>39</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="F12"/>
     </x:row>
     <x:row r="13" ht="13.05" customHeight="1">
       <x:c r="A13" s="9" t="s">
-        <x:v>40</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="B13" s="9" t="s">
-        <x:v>36</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="C13" s="9" t="s">
-        <x:v>15</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D13" s="13"/>
       <x:c r="E13" s="9" t="s">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="F13"/>
     </x:row>
     <x:row r="14" ht="13.05" customHeight="1">
       <x:c r="A14" s="9" t="s">
-        <x:v>42</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="B14" s="9" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="C14" s="9" t="s">
         <x:v>18</x:v>
-      </x:c>
-      <x:c r="C14" s="9" t="s">
-        <x:v>15</x:v>
       </x:c>
       <x:c r="D14" s="13"/>
       <x:c r="E14" s="9" t="s">
-        <x:v>43</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="F14"/>
     </x:row>
     <x:row r="15" ht="13.05" customHeight="1">
       <x:c r="A15" s="9" t="s">
-        <x:v>44</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="B15" s="9" t="s">
-        <x:v>6</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C15" s="9" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D15" s="12" t="n">
-        <x:v>45939</x:v>
-      </x:c>
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D15" s="13"/>
       <x:c r="E15" s="9" t="s">
-        <x:v>45</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="F15"/>
     </x:row>
     <x:row r="16" ht="13.05" customHeight="1">
       <x:c r="A16" s="9" t="s">
-        <x:v>46</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="B16" s="9" t="s">
-        <x:v>10</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="C16" s="9" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="D16" s="13"/>
+      <x:c r="D16" s="12" t="n">
+        <x:v>45939</x:v>
+      </x:c>
       <x:c r="E16" s="9" t="s">
-        <x:v>47</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="F16"/>
     </x:row>
     <x:row r="17" ht="13.05" customHeight="1">
       <x:c r="A17" s="9" t="s">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="B17" s="9" t="s">
-        <x:v>36</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="C17" s="9" t="s">
-        <x:v>23</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D17" s="13"/>
       <x:c r="E17" s="9" t="s">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="F17"/>
     </x:row>
     <x:row r="18" ht="13.05" customHeight="1">
       <x:c r="A18" s="9" t="s">
-        <x:v>50</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="B18" s="9" t="s">
-        <x:v>33</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="C18" s="9" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D18" s="12" t="n">
-        <x:v>45946</x:v>
-      </x:c>
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="D18" s="13"/>
       <x:c r="E18" s="9" t="s">
-        <x:v>51</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="F18"/>
     </x:row>
     <x:row r="19" ht="13.05" customHeight="1">
       <x:c r="A19" s="9" t="s">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="B19" s="9" t="s">
-        <x:v>33</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="C19" s="9" t="s">
-        <x:v>19</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D19" s="12" t="n">
-        <x:v>45959</x:v>
+        <x:v>45946</x:v>
       </x:c>
       <x:c r="E19" s="9" t="s">
-        <x:v>53</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="F19"/>
     </x:row>
     <x:row r="20" ht="13.05" customHeight="1">
       <x:c r="A20" s="9" t="s">
-        <x:v>54</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="B20" s="9" t="s">
         <x:v>36</x:v>
       </x:c>
       <x:c r="C20" s="9" t="s">
-        <x:v>19</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="D20" s="12" t="n">
-        <x:v>45954</x:v>
+        <x:v>45959</x:v>
       </x:c>
       <x:c r="E20" s="9" t="s">
-        <x:v>55</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="F20"/>
     </x:row>
     <x:row r="21" ht="13.05" customHeight="1">
       <x:c r="A21" s="9" t="s">
-        <x:v>56</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="B21" s="9" t="s">
-        <x:v>57</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="C21" s="9" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="D21" s="13"/>
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D21" s="12" t="n">
+        <x:v>45954</x:v>
+      </x:c>
       <x:c r="E21" s="9" t="s">
         <x:v>58</x:v>
       </x:c>
@@ -685,26 +693,26 @@
         <x:v>59</x:v>
       </x:c>
       <x:c r="B22" s="9" t="s">
-        <x:v>33</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="C22" s="9" t="s">
-        <x:v>15</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="D22" s="13"/>
       <x:c r="E22" s="9" t="s">
-        <x:v>60</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="F22"/>
     </x:row>
     <x:row r="23" ht="13.05" customHeight="1">
       <x:c r="A23" s="9" t="s">
-        <x:v>61</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="B23" s="9" t="s">
-        <x:v>62</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="C23" s="9" t="s">
-        <x:v>19</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D23" s="13"/>
       <x:c r="E23" s="9" t="s">
@@ -717,10 +725,10 @@
         <x:v>64</x:v>
       </x:c>
       <x:c r="B24" s="9" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="C24" s="9" t="s">
         <x:v>22</x:v>
-      </x:c>
-      <x:c r="C24" s="9" t="s">
-        <x:v>23</x:v>
       </x:c>
       <x:c r="D24" s="13"/>
       <x:c r="E24" s="9" t="s">
@@ -733,36 +741,52 @@
         <x:v>66</x:v>
       </x:c>
       <x:c r="B25" s="9" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="C25" s="9" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="C25" s="9" t="s">
+      <x:c r="D25" s="13"/>
+      <x:c r="E25" s="9" t="s">
         <x:v>67</x:v>
-      </x:c>
-      <x:c r="D25" s="12" t="n">
-        <x:v>45932</x:v>
-      </x:c>
-      <x:c r="E25" s="9" t="s">
-        <x:v>68</x:v>
       </x:c>
       <x:c r="F25"/>
     </x:row>
     <x:row r="26" ht="13.05" customHeight="1">
       <x:c r="A26" s="9" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="B26" s="9" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="C26" s="9" t="s">
         <x:v>69</x:v>
       </x:c>
-      <x:c r="B26" s="9" t="s">
+      <x:c r="D26" s="12" t="n">
+        <x:v>45932</x:v>
+      </x:c>
+      <x:c r="E26" s="9" t="s">
         <x:v>70</x:v>
       </x:c>
-      <x:c r="C26" s="9" t="s">
-        <x:v>67</x:v>
-      </x:c>
-      <x:c r="D26" s="12" t="n">
+      <x:c r="F26"/>
+    </x:row>
+    <x:row r="27" ht="13.05" customHeight="1">
+      <x:c r="A27" s="9" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="B27" s="9" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="C27" s="9" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="D27" s="12" t="n">
         <x:v>45954</x:v>
       </x:c>
-      <x:c r="E26" s="9" t="s">
-        <x:v>71</x:v>
-      </x:c>
-      <x:c r="F26"/>
+      <x:c r="E27" s="9" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="F27"/>
     </x:row>
   </x:sheetData>
   <x:pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
One-click update from Van Paper 07:22 AM on 2025-11-06
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -67,48 +67,48 @@
     <x:t>McGivern, Kelly W</x:t>
   </x:si>
   <x:si>
+    <x:t>023</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008313</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HB CLE 2407 LORAIN LLC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ballman, John W</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008317</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FRIENDS OF ANSELM HOUSE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Steiner, Owen A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>015</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008318</x:t>
+  </x:si>
+  <x:si>
+    <x:t>WALLACE CARLSON PRINTING</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Bloch, Lea L</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008320</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SEVEN HILLS PREP ACADEMY</x:t>
+  </x:si>
+  <x:si>
     <x:t>040</x:t>
   </x:si>
   <x:si>
-    <x:t>0008313</x:t>
-  </x:si>
-  <x:si>
-    <x:t>HB CLE 2407 LORAIN LLC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Ballman, John W</x:t>
-  </x:si>
-  <x:si>
-    <x:t>023</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0008317</x:t>
-  </x:si>
-  <x:si>
-    <x:t>FRIENDS OF ANSELM HOUSE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Steiner, Owen A</x:t>
-  </x:si>
-  <x:si>
-    <x:t>015</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0008318</x:t>
-  </x:si>
-  <x:si>
-    <x:t>WALLACE CARLSON PRINTING</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Bloch, Lea L</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0008320</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SEVEN HILLS PREP ACADEMY</x:t>
-  </x:si>
-  <x:si>
     <x:t>0008321</x:t>
   </x:si>
   <x:si>
@@ -217,6 +217,15 @@
     <x:t>0008352</x:t>
   </x:si>
   <x:si>
+    <x:t>PETE AND PORKY BIG GAME</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Monroe, Michael D</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008359</x:t>
+  </x:si>
+  <x:si>
     <x:t>HOLY FAMILY MARONITE CHURCH</x:t>
   </x:si>
   <x:si>
@@ -227,9 +236,6 @@
   </x:si>
   <x:si>
     <x:t>SCHMITT MUSIC CTR</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Monroe, Michael D</x:t>
   </x:si>
   <x:si>
     <x:t>0005169</x:t>
@@ -318,7 +324,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:F27"/>
+  <x:dimension ref="A1:F28"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -414,7 +420,9 @@
       <x:c r="C5" s="9" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="D5" s="13"/>
+      <x:c r="D5" s="12" t="n">
+        <x:v>45965</x:v>
+      </x:c>
       <x:c r="E5" s="9" t="s">
         <x:v>19</x:v>
       </x:c>
@@ -428,57 +436,57 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="C6" s="9" t="s">
-        <x:v>22</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D6" s="13"/>
       <x:c r="E6" s="9" t="s">
-        <x:v>23</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F6"/>
     </x:row>
     <x:row r="7" ht="13.05" customHeight="1">
       <x:c r="A7" s="9" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B7" s="9" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="B7" s="9" t="s">
+      <x:c r="C7" s="9" t="s">
         <x:v>25</x:v>
-      </x:c>
-      <x:c r="C7" s="9" t="s">
-        <x:v>26</x:v>
       </x:c>
       <x:c r="D7" s="13"/>
       <x:c r="E7" s="9" t="s">
-        <x:v>27</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="F7"/>
     </x:row>
     <x:row r="8" ht="13.05" customHeight="1">
       <x:c r="A8" s="9" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="B8" s="9" t="s">
         <x:v>28</x:v>
       </x:c>
-      <x:c r="B8" s="9" t="s">
-        <x:v>29</x:v>
-      </x:c>
       <x:c r="C8" s="9" t="s">
-        <x:v>26</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="D8" s="12" t="n">
         <x:v>45929</x:v>
       </x:c>
       <x:c r="E8" s="9" t="s">
-        <x:v>30</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="F8"/>
     </x:row>
     <x:row r="9" ht="13.05" customHeight="1">
       <x:c r="A9" s="9" t="s">
-        <x:v>31</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="B9" s="9" t="s">
         <x:v>21</x:v>
       </x:c>
       <x:c r="C9" s="9" t="s">
-        <x:v>18</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="D9" s="13"/>
       <x:c r="E9" s="9" t="s">
@@ -491,10 +499,10 @@
         <x:v>33</x:v>
       </x:c>
       <x:c r="B10" s="9" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="C10" s="9" t="s">
         <x:v>25</x:v>
-      </x:c>
-      <x:c r="C10" s="9" t="s">
-        <x:v>26</x:v>
       </x:c>
       <x:c r="D10" s="12" t="n">
         <x:v>45950</x:v>
@@ -512,7 +520,7 @@
         <x:v>36</x:v>
       </x:c>
       <x:c r="C11" s="9" t="s">
-        <x:v>18</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="D11" s="13"/>
       <x:c r="E11" s="9" t="s">
@@ -528,7 +536,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="C12" s="9" t="s">
-        <x:v>18</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="D12" s="13"/>
       <x:c r="E12" s="9" t="s">
@@ -544,7 +552,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="C13" s="9" t="s">
-        <x:v>18</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="D13" s="13"/>
       <x:c r="E13" s="9" t="s">
@@ -560,7 +568,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="C14" s="9" t="s">
-        <x:v>18</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="D14" s="13"/>
       <x:c r="E14" s="9" t="s">
@@ -576,7 +584,7 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="C15" s="9" t="s">
-        <x:v>18</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="D15" s="13"/>
       <x:c r="E15" s="9" t="s">
@@ -626,9 +634,11 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="C18" s="9" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="D18" s="13"/>
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="D18" s="12" t="n">
+        <x:v>45965</x:v>
+      </x:c>
       <x:c r="E18" s="9" t="s">
         <x:v>52</x:v>
       </x:c>
@@ -660,7 +670,7 @@
         <x:v>36</x:v>
       </x:c>
       <x:c r="C20" s="9" t="s">
-        <x:v>22</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D20" s="12" t="n">
         <x:v>45959</x:v>
@@ -678,7 +688,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="C21" s="9" t="s">
-        <x:v>22</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D21" s="12" t="n">
         <x:v>45954</x:v>
@@ -696,7 +706,7 @@
         <x:v>60</x:v>
       </x:c>
       <x:c r="C22" s="9" t="s">
-        <x:v>26</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="D22" s="13"/>
       <x:c r="E22" s="9" t="s">
@@ -712,7 +722,7 @@
         <x:v>36</x:v>
       </x:c>
       <x:c r="C23" s="9" t="s">
-        <x:v>18</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="D23" s="13"/>
       <x:c r="E23" s="9" t="s">
@@ -728,9 +738,11 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="C24" s="9" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="D24" s="13"/>
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D24" s="12" t="n">
+        <x:v>45965</x:v>
+      </x:c>
       <x:c r="E24" s="9" t="s">
         <x:v>65</x:v>
       </x:c>
@@ -741,10 +753,10 @@
         <x:v>66</x:v>
       </x:c>
       <x:c r="B25" s="9" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="C25" s="9" t="s">
         <x:v>25</x:v>
-      </x:c>
-      <x:c r="C25" s="9" t="s">
-        <x:v>26</x:v>
       </x:c>
       <x:c r="D25" s="13"/>
       <x:c r="E25" s="9" t="s">
@@ -757,13 +769,13 @@
         <x:v>68</x:v>
       </x:c>
       <x:c r="B26" s="9" t="s">
-        <x:v>29</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="C26" s="9" t="s">
-        <x:v>69</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D26" s="12" t="n">
-        <x:v>45932</x:v>
+        <x:v>45966</x:v>
       </x:c>
       <x:c r="E26" s="9" t="s">
         <x:v>70</x:v>
@@ -775,18 +787,36 @@
         <x:v>71</x:v>
       </x:c>
       <x:c r="B27" s="9" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C27" s="9" t="s">
         <x:v>72</x:v>
       </x:c>
-      <x:c r="C27" s="9" t="s">
-        <x:v>69</x:v>
-      </x:c>
       <x:c r="D27" s="12" t="n">
-        <x:v>45954</x:v>
+        <x:v>45932</x:v>
       </x:c>
       <x:c r="E27" s="9" t="s">
         <x:v>73</x:v>
       </x:c>
       <x:c r="F27"/>
+    </x:row>
+    <x:row r="28" ht="13.05" customHeight="1">
+      <x:c r="A28" s="9" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="B28" s="9" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="C28" s="9" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="D28" s="12" t="n">
+        <x:v>45954</x:v>
+      </x:c>
+      <x:c r="E28" s="9" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="F28"/>
     </x:row>
   </x:sheetData>
   <x:pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
One-click update from Van Paper 07:10 AM on 2025-11-10
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -199,7 +199,7 @@
     <x:t>0008345</x:t>
   </x:si>
   <x:si>
-    <x:t>SLAPSTIX</x:t>
+    <x:t>WOODBURY ICE</x:t>
   </x:si>
   <x:si>
     <x:t>0008347</x:t>
@@ -620,7 +620,9 @@
       <x:c r="C17" s="9" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="D17" s="13"/>
+      <x:c r="D17" s="12" t="n">
+        <x:v>45968</x:v>
+      </x:c>
       <x:c r="E17" s="9" t="s">
         <x:v>50</x:v>
       </x:c>
@@ -722,9 +724,11 @@
         <x:v>36</x:v>
       </x:c>
       <x:c r="C23" s="9" t="s">
-        <x:v>31</x:v>
-      </x:c>
-      <x:c r="D23" s="13"/>
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D23" s="12" t="n">
+        <x:v>45968</x:v>
+      </x:c>
       <x:c r="E23" s="9" t="s">
         <x:v>63</x:v>
       </x:c>

</xml_diff>

<commit_message>
One-click update from Van Paper 07:26 AM on 2025-11-11
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -224,6 +224,12 @@
   </x:si>
   <x:si>
     <x:t>0008359</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NATURE PATHWAYS ELC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008366</x:t>
   </x:si>
   <x:si>
     <x:t>HOLY FAMILY MARONITE CHURCH</x:t>
@@ -324,7 +330,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:F28"/>
+  <x:dimension ref="A1:F29"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -454,7 +460,9 @@
       <x:c r="C7" s="9" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="D7" s="13"/>
+      <x:c r="D7" s="12" t="n">
+        <x:v>45971</x:v>
+      </x:c>
       <x:c r="E7" s="9" t="s">
         <x:v>26</x:v>
       </x:c>
@@ -791,36 +799,52 @@
         <x:v>71</x:v>
       </x:c>
       <x:c r="B27" s="9" t="s">
-        <x:v>28</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="C27" s="9" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="D27" s="13"/>
+      <x:c r="E27" s="9" t="s">
         <x:v>72</x:v>
-      </x:c>
-      <x:c r="D27" s="12" t="n">
-        <x:v>45932</x:v>
-      </x:c>
-      <x:c r="E27" s="9" t="s">
-        <x:v>73</x:v>
       </x:c>
       <x:c r="F27"/>
     </x:row>
     <x:row r="28" ht="13.05" customHeight="1">
       <x:c r="A28" s="9" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="B28" s="9" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C28" s="9" t="s">
         <x:v>74</x:v>
       </x:c>
-      <x:c r="B28" s="9" t="s">
-        <x:v>69</x:v>
-      </x:c>
-      <x:c r="C28" s="9" t="s">
-        <x:v>72</x:v>
-      </x:c>
       <x:c r="D28" s="12" t="n">
-        <x:v>45954</x:v>
+        <x:v>45932</x:v>
       </x:c>
       <x:c r="E28" s="9" t="s">
         <x:v>75</x:v>
       </x:c>
       <x:c r="F28"/>
+    </x:row>
+    <x:row r="29" ht="13.05" customHeight="1">
+      <x:c r="A29" s="9" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="B29" s="9" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="C29" s="9" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="D29" s="12" t="n">
+        <x:v>45954</x:v>
+      </x:c>
+      <x:c r="E29" s="9" t="s">
+        <x:v>77</x:v>
+      </x:c>
+      <x:c r="F29"/>
     </x:row>
   </x:sheetData>
   <x:pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
One-click update from Van Paper 07:10 AM on 2025-11-12
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -230,6 +230,12 @@
   </x:si>
   <x:si>
     <x:t>0008366</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NICOLLET COURT RETAIL MALL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008368</x:t>
   </x:si>
   <x:si>
     <x:t>HOLY FAMILY MARONITE CHURCH</x:t>
@@ -330,7 +336,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:F29"/>
+  <x:dimension ref="A1:F30"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -815,36 +821,52 @@
         <x:v>73</x:v>
       </x:c>
       <x:c r="B28" s="9" t="s">
-        <x:v>28</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C28" s="9" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="D28" s="13"/>
+      <x:c r="E28" s="9" t="s">
         <x:v>74</x:v>
-      </x:c>
-      <x:c r="D28" s="12" t="n">
-        <x:v>45932</x:v>
-      </x:c>
-      <x:c r="E28" s="9" t="s">
-        <x:v>75</x:v>
       </x:c>
       <x:c r="F28"/>
     </x:row>
     <x:row r="29" ht="13.05" customHeight="1">
       <x:c r="A29" s="9" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="B29" s="9" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C29" s="9" t="s">
         <x:v>76</x:v>
       </x:c>
-      <x:c r="B29" s="9" t="s">
-        <x:v>69</x:v>
-      </x:c>
-      <x:c r="C29" s="9" t="s">
-        <x:v>74</x:v>
-      </x:c>
       <x:c r="D29" s="12" t="n">
-        <x:v>45954</x:v>
+        <x:v>45932</x:v>
       </x:c>
       <x:c r="E29" s="9" t="s">
         <x:v>77</x:v>
       </x:c>
       <x:c r="F29"/>
+    </x:row>
+    <x:row r="30" ht="13.05" customHeight="1">
+      <x:c r="A30" s="9" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="B30" s="9" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="C30" s="9" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="D30" s="12" t="n">
+        <x:v>45954</x:v>
+      </x:c>
+      <x:c r="E30" s="9" t="s">
+        <x:v>79</x:v>
+      </x:c>
+      <x:c r="F30"/>
     </x:row>
   </x:sheetData>
   <x:pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
One-click update from Van Paper 07:23 AM on 2025-11-13
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -232,10 +232,16 @@
     <x:t>0008366</x:t>
   </x:si>
   <x:si>
-    <x:t>NICOLLET COURT RETAIL MALL</x:t>
+    <x:t>NICOLLET RETAIL LLC</x:t>
   </x:si>
   <x:si>
     <x:t>0008368</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MAYNARD'S</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008369</x:t>
   </x:si>
   <x:si>
     <x:t>HOLY FAMILY MARONITE CHURCH</x:t>
@@ -336,7 +342,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:F30"/>
+  <x:dimension ref="A1:F31"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -824,7 +830,7 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="C28" s="9" t="s">
-        <x:v>25</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D28" s="13"/>
       <x:c r="E28" s="9" t="s">
@@ -837,36 +843,52 @@
         <x:v>75</x:v>
       </x:c>
       <x:c r="B29" s="9" t="s">
-        <x:v>28</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="C29" s="9" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="D29" s="13"/>
+      <x:c r="E29" s="9" t="s">
         <x:v>76</x:v>
-      </x:c>
-      <x:c r="D29" s="12" t="n">
-        <x:v>45932</x:v>
-      </x:c>
-      <x:c r="E29" s="9" t="s">
-        <x:v>77</x:v>
       </x:c>
       <x:c r="F29"/>
     </x:row>
     <x:row r="30" ht="13.05" customHeight="1">
       <x:c r="A30" s="9" t="s">
+        <x:v>77</x:v>
+      </x:c>
+      <x:c r="B30" s="9" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C30" s="9" t="s">
         <x:v>78</x:v>
       </x:c>
-      <x:c r="B30" s="9" t="s">
-        <x:v>69</x:v>
-      </x:c>
-      <x:c r="C30" s="9" t="s">
-        <x:v>76</x:v>
-      </x:c>
       <x:c r="D30" s="12" t="n">
-        <x:v>45954</x:v>
+        <x:v>45932</x:v>
       </x:c>
       <x:c r="E30" s="9" t="s">
         <x:v>79</x:v>
       </x:c>
       <x:c r="F30"/>
+    </x:row>
+    <x:row r="31" ht="13.05" customHeight="1">
+      <x:c r="A31" s="9" t="s">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="B31" s="9" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="C31" s="9" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="D31" s="12" t="n">
+        <x:v>45954</x:v>
+      </x:c>
+      <x:c r="E31" s="9" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="F31"/>
     </x:row>
   </x:sheetData>
   <x:pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
One-click update from Van Paper 07:11 AM on 2025-11-14
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -242,6 +242,12 @@
   </x:si>
   <x:si>
     <x:t>0008369</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DG PROCESSING</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008370</x:t>
   </x:si>
   <x:si>
     <x:t>HOLY FAMILY MARONITE CHURCH</x:t>
@@ -342,7 +348,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:F31"/>
+  <x:dimension ref="A1:F32"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -859,36 +865,52 @@
         <x:v>77</x:v>
       </x:c>
       <x:c r="B30" s="9" t="s">
-        <x:v>28</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="C30" s="9" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D30" s="13"/>
+      <x:c r="E30" s="9" t="s">
         <x:v>78</x:v>
-      </x:c>
-      <x:c r="D30" s="12" t="n">
-        <x:v>45932</x:v>
-      </x:c>
-      <x:c r="E30" s="9" t="s">
-        <x:v>79</x:v>
       </x:c>
       <x:c r="F30"/>
     </x:row>
     <x:row r="31" ht="13.05" customHeight="1">
       <x:c r="A31" s="9" t="s">
+        <x:v>79</x:v>
+      </x:c>
+      <x:c r="B31" s="9" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C31" s="9" t="s">
         <x:v>80</x:v>
       </x:c>
-      <x:c r="B31" s="9" t="s">
-        <x:v>69</x:v>
-      </x:c>
-      <x:c r="C31" s="9" t="s">
-        <x:v>78</x:v>
-      </x:c>
       <x:c r="D31" s="12" t="n">
-        <x:v>45954</x:v>
+        <x:v>45932</x:v>
       </x:c>
       <x:c r="E31" s="9" t="s">
         <x:v>81</x:v>
       </x:c>
       <x:c r="F31"/>
+    </x:row>
+    <x:row r="32" ht="13.05" customHeight="1">
+      <x:c r="A32" s="9" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="B32" s="9" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="C32" s="9" t="s">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="D32" s="12" t="n">
+        <x:v>45954</x:v>
+      </x:c>
+      <x:c r="E32" s="9" t="s">
+        <x:v>83</x:v>
+      </x:c>
+      <x:c r="F32"/>
     </x:row>
   </x:sheetData>
   <x:pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
One-click update from Van Paper 07:06 AM on 2025-11-17
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -248,6 +248,21 @@
   </x:si>
   <x:si>
     <x:t>0008370</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DAN'S DEER PROCESSING</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Van, Kyle C</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008371</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HOLIDAY INN EXPRESS &amp; SUITES</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008372</x:t>
   </x:si>
   <x:si>
     <x:t>HOLY FAMILY MARONITE CHURCH</x:t>
@@ -348,7 +363,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:F32"/>
+  <x:dimension ref="A1:F34"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -881,14 +896,12 @@
         <x:v>79</x:v>
       </x:c>
       <x:c r="B31" s="9" t="s">
-        <x:v>28</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="C31" s="9" t="s">
-        <x:v>80</x:v>
-      </x:c>
-      <x:c r="D31" s="12" t="n">
-        <x:v>45932</x:v>
-      </x:c>
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D31" s="13"/>
       <x:c r="E31" s="9" t="s">
         <x:v>81</x:v>
       </x:c>
@@ -899,18 +912,52 @@
         <x:v>82</x:v>
       </x:c>
       <x:c r="B32" s="9" t="s">
-        <x:v>69</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="C32" s="9" t="s">
-        <x:v>80</x:v>
-      </x:c>
-      <x:c r="D32" s="12" t="n">
-        <x:v>45954</x:v>
-      </x:c>
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D32" s="13"/>
       <x:c r="E32" s="9" t="s">
         <x:v>83</x:v>
       </x:c>
       <x:c r="F32"/>
+    </x:row>
+    <x:row r="33" ht="13.05" customHeight="1">
+      <x:c r="A33" s="9" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="B33" s="9" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C33" s="9" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="D33" s="12" t="n">
+        <x:v>45932</x:v>
+      </x:c>
+      <x:c r="E33" s="9" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="F33"/>
+    </x:row>
+    <x:row r="34" ht="13.05" customHeight="1">
+      <x:c r="A34" s="9" t="s">
+        <x:v>87</x:v>
+      </x:c>
+      <x:c r="B34" s="9" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="C34" s="9" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="D34" s="12" t="n">
+        <x:v>45954</x:v>
+      </x:c>
+      <x:c r="E34" s="9" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="F34"/>
     </x:row>
   </x:sheetData>
   <x:pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
One-click update from Van Paper 07:27 AM on 2025-11-18
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -917,7 +917,9 @@
       <x:c r="C32" s="9" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="D32" s="13"/>
+      <x:c r="D32" s="12" t="n">
+        <x:v>45978</x:v>
+      </x:c>
       <x:c r="E32" s="9" t="s">
         <x:v>83</x:v>
       </x:c>

</xml_diff>

<commit_message>
One-click update from Van Paper 07:06 AM on 2025-11-19
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -58,6 +58,9 @@
     <x:t>Cina, Jonathan D</x:t>
   </x:si>
   <x:si>
+    <x:t>023</x:t>
+  </x:si>
+  <x:si>
     <x:t>0008303</x:t>
   </x:si>
   <x:si>
@@ -67,9 +70,6 @@
     <x:t>McGivern, Kelly W</x:t>
   </x:si>
   <x:si>
-    <x:t>023</x:t>
-  </x:si>
-  <x:si>
     <x:t>0008313</x:t>
   </x:si>
   <x:si>
@@ -263,6 +263,12 @@
   </x:si>
   <x:si>
     <x:t>0008372</x:t>
+  </x:si>
+  <x:si>
+    <x:t>REBECCA'S BAKERY &amp; CAFE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008374</x:t>
   </x:si>
   <x:si>
     <x:t>HOLY FAMILY MARONITE CHURCH</x:t>
@@ -363,7 +369,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:F34"/>
+  <x:dimension ref="A1:F35"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -439,25 +445,25 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="C4" s="9" t="s">
-        <x:v>7</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="D4" s="12" t="n">
         <x:v>45960</x:v>
       </x:c>
       <x:c r="E4" s="9" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="F4"/>
     </x:row>
     <x:row r="5" ht="13.05" customHeight="1">
       <x:c r="A5" s="9" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="B5" s="9" t="s">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="C5" s="9" t="s">
-        <x:v>18</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="D5" s="12" t="n">
         <x:v>45965</x:v>
@@ -475,7 +481,7 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="C6" s="9" t="s">
-        <x:v>18</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="D6" s="13"/>
       <x:c r="E6" s="9" t="s">
@@ -713,7 +719,7 @@
         <x:v>36</x:v>
       </x:c>
       <x:c r="C20" s="9" t="s">
-        <x:v>18</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="D20" s="12" t="n">
         <x:v>45959</x:v>
@@ -731,7 +737,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="C21" s="9" t="s">
-        <x:v>18</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="D21" s="12" t="n">
         <x:v>45954</x:v>
@@ -765,7 +771,7 @@
         <x:v>36</x:v>
       </x:c>
       <x:c r="C23" s="9" t="s">
-        <x:v>18</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="D23" s="12" t="n">
         <x:v>45968</x:v>
@@ -783,7 +789,7 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="C24" s="9" t="s">
-        <x:v>18</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="D24" s="12" t="n">
         <x:v>45965</x:v>
@@ -851,9 +857,11 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="C28" s="9" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="D28" s="13"/>
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="D28" s="12" t="n">
+        <x:v>45979</x:v>
+      </x:c>
       <x:c r="E28" s="9" t="s">
         <x:v>74</x:v>
       </x:c>
@@ -901,7 +909,9 @@
       <x:c r="C31" s="9" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="D31" s="13"/>
+      <x:c r="D31" s="12" t="n">
+        <x:v>45979</x:v>
+      </x:c>
       <x:c r="E31" s="9" t="s">
         <x:v>81</x:v>
       </x:c>
@@ -930,36 +940,52 @@
         <x:v>84</x:v>
       </x:c>
       <x:c r="B33" s="9" t="s">
-        <x:v>28</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="C33" s="9" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D33" s="13"/>
+      <x:c r="E33" s="9" t="s">
         <x:v>85</x:v>
-      </x:c>
-      <x:c r="D33" s="12" t="n">
-        <x:v>45932</x:v>
-      </x:c>
-      <x:c r="E33" s="9" t="s">
-        <x:v>86</x:v>
       </x:c>
       <x:c r="F33"/>
     </x:row>
     <x:row r="34" ht="13.05" customHeight="1">
       <x:c r="A34" s="9" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="B34" s="9" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C34" s="9" t="s">
         <x:v>87</x:v>
       </x:c>
-      <x:c r="B34" s="9" t="s">
-        <x:v>69</x:v>
-      </x:c>
-      <x:c r="C34" s="9" t="s">
-        <x:v>85</x:v>
-      </x:c>
       <x:c r="D34" s="12" t="n">
-        <x:v>45954</x:v>
+        <x:v>45932</x:v>
       </x:c>
       <x:c r="E34" s="9" t="s">
         <x:v>88</x:v>
       </x:c>
       <x:c r="F34"/>
+    </x:row>
+    <x:row r="35" ht="13.05" customHeight="1">
+      <x:c r="A35" s="9" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="B35" s="9" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="C35" s="9" t="s">
+        <x:v>87</x:v>
+      </x:c>
+      <x:c r="D35" s="12" t="n">
+        <x:v>45954</x:v>
+      </x:c>
+      <x:c r="E35" s="9" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="F35"/>
     </x:row>
   </x:sheetData>
   <x:pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
One-click update from Van Paper 07:23 AM on 2025-11-20
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -269,6 +269,18 @@
   </x:si>
   <x:si>
     <x:t>0008374</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SMALL HOURS LLC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008375</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">YELLOW BRICK ROAD CHILD CARE </x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008376</x:t>
   </x:si>
   <x:si>
     <x:t>HOLY FAMILY MARONITE CHURCH</x:t>
@@ -369,7 +381,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:F35"/>
+  <x:dimension ref="A1:F37"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -945,7 +957,9 @@
       <x:c r="C33" s="9" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="D33" s="13"/>
+      <x:c r="D33" s="12" t="n">
+        <x:v>45980</x:v>
+      </x:c>
       <x:c r="E33" s="9" t="s">
         <x:v>85</x:v>
       </x:c>
@@ -956,36 +970,68 @@
         <x:v>86</x:v>
       </x:c>
       <x:c r="B34" s="9" t="s">
-        <x:v>28</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="C34" s="9" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D34" s="13"/>
+      <x:c r="E34" s="9" t="s">
         <x:v>87</x:v>
-      </x:c>
-      <x:c r="D34" s="12" t="n">
-        <x:v>45932</x:v>
-      </x:c>
-      <x:c r="E34" s="9" t="s">
-        <x:v>88</x:v>
       </x:c>
       <x:c r="F34"/>
     </x:row>
     <x:row r="35" ht="13.05" customHeight="1">
       <x:c r="A35" s="9" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="B35" s="9" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="C35" s="9" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="D35" s="13"/>
+      <x:c r="E35" s="9" t="s">
         <x:v>89</x:v>
       </x:c>
-      <x:c r="B35" s="9" t="s">
+      <x:c r="F35"/>
+    </x:row>
+    <x:row r="36" ht="13.05" customHeight="1">
+      <x:c r="A36" s="9" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="B36" s="9" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C36" s="9" t="s">
+        <x:v>91</x:v>
+      </x:c>
+      <x:c r="D36" s="12" t="n">
+        <x:v>45932</x:v>
+      </x:c>
+      <x:c r="E36" s="9" t="s">
+        <x:v>92</x:v>
+      </x:c>
+      <x:c r="F36"/>
+    </x:row>
+    <x:row r="37" ht="13.05" customHeight="1">
+      <x:c r="A37" s="9" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="B37" s="9" t="s">
         <x:v>69</x:v>
       </x:c>
-      <x:c r="C35" s="9" t="s">
-        <x:v>87</x:v>
-      </x:c>
-      <x:c r="D35" s="12" t="n">
+      <x:c r="C37" s="9" t="s">
+        <x:v>91</x:v>
+      </x:c>
+      <x:c r="D37" s="12" t="n">
         <x:v>45954</x:v>
       </x:c>
-      <x:c r="E35" s="9" t="s">
-        <x:v>90</x:v>
-      </x:c>
-      <x:c r="F35"/>
+      <x:c r="E37" s="9" t="s">
+        <x:v>94</x:v>
+      </x:c>
+      <x:c r="F37"/>
     </x:row>
   </x:sheetData>
   <x:pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
One-click update from Van Paper 07:27 AM on 2025-11-25
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -850,7 +850,7 @@
         <x:v>71</x:v>
       </x:c>
       <x:c r="B27" s="9" t="s">
-        <x:v>6</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C27" s="9" t="s">
         <x:v>25</x:v>
@@ -991,7 +991,9 @@
       <x:c r="C35" s="9" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="D35" s="13"/>
+      <x:c r="D35" s="12" t="n">
+        <x:v>45985</x:v>
+      </x:c>
       <x:c r="E35" s="9" t="s">
         <x:v>89</x:v>
       </x:c>

</xml_diff>

<commit_message>
One-click update from Van Paper 07:05 AM on 2025-12-01
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -855,7 +855,9 @@
       <x:c r="C27" s="9" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="D27" s="13"/>
+      <x:c r="D27" s="12" t="n">
+        <x:v>45987</x:v>
+      </x:c>
       <x:c r="E27" s="9" t="s">
         <x:v>72</x:v>
       </x:c>

</xml_diff>

<commit_message>
One-click update from Van Paper 07:06 AM on 2025-12-03
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -281,6 +281,12 @@
   </x:si>
   <x:si>
     <x:t>0008376</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MERWIN LIQUORS FALCON HEIGHTS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008384</x:t>
   </x:si>
   <x:si>
     <x:t>HOLY FAMILY MARONITE CHURCH</x:t>
@@ -381,7 +387,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:F37"/>
+  <x:dimension ref="A1:F38"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -1006,36 +1012,52 @@
         <x:v>90</x:v>
       </x:c>
       <x:c r="B36" s="9" t="s">
-        <x:v>28</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="C36" s="9" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="D36" s="13"/>
+      <x:c r="E36" s="9" t="s">
         <x:v>91</x:v>
-      </x:c>
-      <x:c r="D36" s="12" t="n">
-        <x:v>45932</x:v>
-      </x:c>
-      <x:c r="E36" s="9" t="s">
-        <x:v>92</x:v>
       </x:c>
       <x:c r="F36"/>
     </x:row>
     <x:row r="37" ht="13.05" customHeight="1">
       <x:c r="A37" s="9" t="s">
+        <x:v>92</x:v>
+      </x:c>
+      <x:c r="B37" s="9" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C37" s="9" t="s">
         <x:v>93</x:v>
       </x:c>
-      <x:c r="B37" s="9" t="s">
-        <x:v>69</x:v>
-      </x:c>
-      <x:c r="C37" s="9" t="s">
-        <x:v>91</x:v>
-      </x:c>
       <x:c r="D37" s="12" t="n">
-        <x:v>45954</x:v>
+        <x:v>45932</x:v>
       </x:c>
       <x:c r="E37" s="9" t="s">
         <x:v>94</x:v>
       </x:c>
       <x:c r="F37"/>
+    </x:row>
+    <x:row r="38" ht="13.05" customHeight="1">
+      <x:c r="A38" s="9" t="s">
+        <x:v>95</x:v>
+      </x:c>
+      <x:c r="B38" s="9" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="C38" s="9" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="D38" s="12" t="n">
+        <x:v>45954</x:v>
+      </x:c>
+      <x:c r="E38" s="9" t="s">
+        <x:v>96</x:v>
+      </x:c>
+      <x:c r="F38"/>
     </x:row>
   </x:sheetData>
   <x:pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
One-click update from Van Paper 07:06 AM on 2025-12-08
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -287,6 +287,12 @@
   </x:si>
   <x:si>
     <x:t>0008384</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HONEYCOMB SALON LLC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008385</x:t>
   </x:si>
   <x:si>
     <x:t>HOLY FAMILY MARONITE CHURCH</x:t>
@@ -387,7 +393,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:F38"/>
+  <x:dimension ref="A1:F39"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -1017,7 +1023,9 @@
       <x:c r="C36" s="9" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="D36" s="13"/>
+      <x:c r="D36" s="12" t="n">
+        <x:v>45996</x:v>
+      </x:c>
       <x:c r="E36" s="9" t="s">
         <x:v>91</x:v>
       </x:c>
@@ -1028,36 +1036,52 @@
         <x:v>92</x:v>
       </x:c>
       <x:c r="B37" s="9" t="s">
-        <x:v>28</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C37" s="9" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="D37" s="13"/>
+      <x:c r="E37" s="9" t="s">
         <x:v>93</x:v>
-      </x:c>
-      <x:c r="D37" s="12" t="n">
-        <x:v>45932</x:v>
-      </x:c>
-      <x:c r="E37" s="9" t="s">
-        <x:v>94</x:v>
       </x:c>
       <x:c r="F37"/>
     </x:row>
     <x:row r="38" ht="13.05" customHeight="1">
       <x:c r="A38" s="9" t="s">
+        <x:v>94</x:v>
+      </x:c>
+      <x:c r="B38" s="9" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C38" s="9" t="s">
         <x:v>95</x:v>
       </x:c>
-      <x:c r="B38" s="9" t="s">
-        <x:v>69</x:v>
-      </x:c>
-      <x:c r="C38" s="9" t="s">
-        <x:v>93</x:v>
-      </x:c>
       <x:c r="D38" s="12" t="n">
-        <x:v>45954</x:v>
+        <x:v>45932</x:v>
       </x:c>
       <x:c r="E38" s="9" t="s">
         <x:v>96</x:v>
       </x:c>
       <x:c r="F38"/>
+    </x:row>
+    <x:row r="39" ht="13.05" customHeight="1">
+      <x:c r="A39" s="9" t="s">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="B39" s="9" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="C39" s="9" t="s">
+        <x:v>95</x:v>
+      </x:c>
+      <x:c r="D39" s="12" t="n">
+        <x:v>45954</x:v>
+      </x:c>
+      <x:c r="E39" s="9" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="F39"/>
     </x:row>
   </x:sheetData>
   <x:pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
One-click update from Van Paper 08:46 AM on 2025-12-23
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -226,7 +226,7 @@
     <x:t>0008359</x:t>
   </x:si>
   <x:si>
-    <x:t>NATURE PATHWAYS ELC</x:t>
+    <x:t>NATURE PATHWAYS EARLY LEARNING</x:t>
   </x:si>
   <x:si>
     <x:t>0008366</x:t>
@@ -289,16 +289,28 @@
     <x:t>0008384</x:t>
   </x:si>
   <x:si>
-    <x:t>HONEYCOMB SALON LLC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0008385</x:t>
+    <x:t>ENDOCRINOLOGY CLINIC OF MPLS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008396</x:t>
+  </x:si>
+  <x:si>
+    <x:t>WOODLANE FLOWERS INC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0004759</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PILGRIM DRY CLEANERS INC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>003</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0004938</x:t>
   </x:si>
   <x:si>
     <x:t>HOLY FAMILY MARONITE CHURCH</x:t>
-  </x:si>
-  <x:si>
-    <x:t>003</x:t>
   </x:si>
   <x:si>
     <x:t>0004965</x:t>
@@ -393,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:F39"/>
+  <x:dimension ref="A1:F41"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -507,7 +519,9 @@
       <x:c r="C6" s="9" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="D6" s="13"/>
+      <x:c r="D6" s="12" t="n">
+        <x:v>46000</x:v>
+      </x:c>
       <x:c r="E6" s="9" t="s">
         <x:v>22</x:v>
       </x:c>
@@ -833,7 +847,9 @@
       <x:c r="C25" s="9" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="D25" s="13"/>
+      <x:c r="D25" s="12" t="n">
+        <x:v>46009</x:v>
+      </x:c>
       <x:c r="E25" s="9" t="s">
         <x:v>67</x:v>
       </x:c>
@@ -865,7 +881,7 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="C27" s="9" t="s">
-        <x:v>25</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="D27" s="12" t="n">
         <x:v>45987</x:v>
@@ -1000,7 +1016,7 @@
         <x:v>88</x:v>
       </x:c>
       <x:c r="B35" s="9" t="s">
-        <x:v>60</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="C35" s="9" t="s">
         <x:v>15</x:v>
@@ -1036,10 +1052,10 @@
         <x:v>92</x:v>
       </x:c>
       <x:c r="B37" s="9" t="s">
-        <x:v>21</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C37" s="9" t="s">
-        <x:v>15</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="D37" s="13"/>
       <x:c r="E37" s="9" t="s">
@@ -1052,36 +1068,72 @@
         <x:v>94</x:v>
       </x:c>
       <x:c r="B38" s="9" t="s">
-        <x:v>28</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="C38" s="9" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D38" s="12" t="n">
+        <x:v>46003</x:v>
+      </x:c>
+      <x:c r="E38" s="9" t="s">
         <x:v>95</x:v>
-      </x:c>
-      <x:c r="D38" s="12" t="n">
-        <x:v>45932</x:v>
-      </x:c>
-      <x:c r="E38" s="9" t="s">
-        <x:v>96</x:v>
       </x:c>
       <x:c r="F38"/>
     </x:row>
     <x:row r="39" ht="13.05" customHeight="1">
       <x:c r="A39" s="9" t="s">
+        <x:v>96</x:v>
+      </x:c>
+      <x:c r="B39" s="9" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="C39" s="9" t="s">
         <x:v>97</x:v>
       </x:c>
-      <x:c r="B39" s="9" t="s">
-        <x:v>69</x:v>
-      </x:c>
-      <x:c r="C39" s="9" t="s">
-        <x:v>95</x:v>
-      </x:c>
       <x:c r="D39" s="12" t="n">
-        <x:v>45954</x:v>
+        <x:v>46006</x:v>
       </x:c>
       <x:c r="E39" s="9" t="s">
         <x:v>98</x:v>
       </x:c>
       <x:c r="F39"/>
+    </x:row>
+    <x:row r="40" ht="13.05" customHeight="1">
+      <x:c r="A40" s="9" t="s">
+        <x:v>99</x:v>
+      </x:c>
+      <x:c r="B40" s="9" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C40" s="9" t="s">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="D40" s="12" t="n">
+        <x:v>45932</x:v>
+      </x:c>
+      <x:c r="E40" s="9" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="F40"/>
+    </x:row>
+    <x:row r="41" ht="13.05" customHeight="1">
+      <x:c r="A41" s="9" t="s">
+        <x:v>101</x:v>
+      </x:c>
+      <x:c r="B41" s="9" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="C41" s="9" t="s">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="D41" s="12" t="n">
+        <x:v>45954</x:v>
+      </x:c>
+      <x:c r="E41" s="9" t="s">
+        <x:v>102</x:v>
+      </x:c>
+      <x:c r="F41"/>
     </x:row>
   </x:sheetData>
   <x:pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
One-click update from Van Paper 07:24 AM on 2025-12-30
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -293,6 +293,12 @@
   </x:si>
   <x:si>
     <x:t>0008396</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NAI LEGACY</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008398</x:t>
   </x:si>
   <x:si>
     <x:t>WOODLANE FLOWERS INC</x:t>
@@ -405,7 +411,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:F41"/>
+  <x:dimension ref="A1:F42"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -1068,14 +1074,12 @@
         <x:v>94</x:v>
       </x:c>
       <x:c r="B38" s="9" t="s">
-        <x:v>10</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C38" s="9" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="D38" s="12" t="n">
-        <x:v>46003</x:v>
-      </x:c>
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="D38" s="13"/>
       <x:c r="E38" s="9" t="s">
         <x:v>95</x:v>
       </x:c>
@@ -1086,31 +1090,31 @@
         <x:v>96</x:v>
       </x:c>
       <x:c r="B39" s="9" t="s">
-        <x:v>24</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="C39" s="9" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D39" s="12" t="n">
+        <x:v>46003</x:v>
+      </x:c>
+      <x:c r="E39" s="9" t="s">
         <x:v>97</x:v>
-      </x:c>
-      <x:c r="D39" s="12" t="n">
-        <x:v>46006</x:v>
-      </x:c>
-      <x:c r="E39" s="9" t="s">
-        <x:v>98</x:v>
       </x:c>
       <x:c r="F39"/>
     </x:row>
     <x:row r="40" ht="13.05" customHeight="1">
       <x:c r="A40" s="9" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="B40" s="9" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="C40" s="9" t="s">
         <x:v>99</x:v>
       </x:c>
-      <x:c r="B40" s="9" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="C40" s="9" t="s">
-        <x:v>97</x:v>
-      </x:c>
       <x:c r="D40" s="12" t="n">
-        <x:v>45932</x:v>
+        <x:v>46006</x:v>
       </x:c>
       <x:c r="E40" s="9" t="s">
         <x:v>100</x:v>
@@ -1122,18 +1126,36 @@
         <x:v>101</x:v>
       </x:c>
       <x:c r="B41" s="9" t="s">
-        <x:v>69</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="C41" s="9" t="s">
-        <x:v>97</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="D41" s="12" t="n">
-        <x:v>45954</x:v>
+        <x:v>45932</x:v>
       </x:c>
       <x:c r="E41" s="9" t="s">
         <x:v>102</x:v>
       </x:c>
       <x:c r="F41"/>
+    </x:row>
+    <x:row r="42" ht="13.05" customHeight="1">
+      <x:c r="A42" s="9" t="s">
+        <x:v>103</x:v>
+      </x:c>
+      <x:c r="B42" s="9" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="C42" s="9" t="s">
+        <x:v>99</x:v>
+      </x:c>
+      <x:c r="D42" s="12" t="n">
+        <x:v>45954</x:v>
+      </x:c>
+      <x:c r="E42" s="9" t="s">
+        <x:v>104</x:v>
+      </x:c>
+      <x:c r="F42"/>
     </x:row>
   </x:sheetData>
   <x:pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
One-click update from Van Paper 07:10 AM on 2026-01-02
</commit_message>
<xml_diff>
--- a/leaderboard_new.xlsx
+++ b/leaderboard_new.xlsx
@@ -295,10 +295,22 @@
     <x:t>0008396</x:t>
   </x:si>
   <x:si>
-    <x:t>NAI LEGACY</x:t>
+    <x:t>TONKA PARTNERS LLC</x:t>
   </x:si>
   <x:si>
     <x:t>0008398</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1655 BEAM LLC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008399</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LIQUOR BARREL CP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0008400</x:t>
   </x:si>
   <x:si>
     <x:t>WOODLANE FLOWERS INC</x:t>
@@ -411,7 +423,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:F42"/>
+  <x:dimension ref="A1:F44"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -1090,14 +1102,12 @@
         <x:v>96</x:v>
       </x:c>
       <x:c r="B39" s="9" t="s">
-        <x:v>10</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C39" s="9" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="D39" s="12" t="n">
-        <x:v>46003</x:v>
-      </x:c>
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="D39" s="13"/>
       <x:c r="E39" s="9" t="s">
         <x:v>97</x:v>
       </x:c>
@@ -1108,54 +1118,88 @@
         <x:v>98</x:v>
       </x:c>
       <x:c r="B40" s="9" t="s">
-        <x:v>24</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="C40" s="9" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="D40" s="13"/>
+      <x:c r="E40" s="9" t="s">
         <x:v>99</x:v>
-      </x:c>
-      <x:c r="D40" s="12" t="n">
-        <x:v>46006</x:v>
-      </x:c>
-      <x:c r="E40" s="9" t="s">
-        <x:v>100</x:v>
       </x:c>
       <x:c r="F40"/>
     </x:row>
     <x:row r="41" ht="13.05" customHeight="1">
       <x:c r="A41" s="9" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="B41" s="9" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="C41" s="9" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D41" s="12" t="n">
+        <x:v>46003</x:v>
+      </x:c>
+      <x:c r="E41" s="9" t="s">
         <x:v>101</x:v>
-      </x:c>
-      <x:c r="B41" s="9" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="C41" s="9" t="s">
-        <x:v>99</x:v>
-      </x:c>
-      <x:c r="D41" s="12" t="n">
-        <x:v>45932</x:v>
-      </x:c>
-      <x:c r="E41" s="9" t="s">
-        <x:v>102</x:v>
       </x:c>
       <x:c r="F41"/>
     </x:row>
     <x:row r="42" ht="13.05" customHeight="1">
       <x:c r="A42" s="9" t="s">
+        <x:v>102</x:v>
+      </x:c>
+      <x:c r="B42" s="9" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="C42" s="9" t="s">
         <x:v>103</x:v>
       </x:c>
-      <x:c r="B42" s="9" t="s">
-        <x:v>69</x:v>
-      </x:c>
-      <x:c r="C42" s="9" t="s">
-        <x:v>99</x:v>
-      </x:c>
       <x:c r="D42" s="12" t="n">
-        <x:v>45954</x:v>
+        <x:v>46006</x:v>
       </x:c>
       <x:c r="E42" s="9" t="s">
         <x:v>104</x:v>
       </x:c>
       <x:c r="F42"/>
+    </x:row>
+    <x:row r="43" ht="13.05" customHeight="1">
+      <x:c r="A43" s="9" t="s">
+        <x:v>105</x:v>
+      </x:c>
+      <x:c r="B43" s="9" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C43" s="9" t="s">
+        <x:v>103</x:v>
+      </x:c>
+      <x:c r="D43" s="12" t="n">
+        <x:v>45932</x:v>
+      </x:c>
+      <x:c r="E43" s="9" t="s">
+        <x:v>106</x:v>
+      </x:c>
+      <x:c r="F43"/>
+    </x:row>
+    <x:row r="44" ht="13.05" customHeight="1">
+      <x:c r="A44" s="9" t="s">
+        <x:v>107</x:v>
+      </x:c>
+      <x:c r="B44" s="9" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="C44" s="9" t="s">
+        <x:v>103</x:v>
+      </x:c>
+      <x:c r="D44" s="12" t="n">
+        <x:v>45954</x:v>
+      </x:c>
+      <x:c r="E44" s="9" t="s">
+        <x:v>108</x:v>
+      </x:c>
+      <x:c r="F44"/>
     </x:row>
   </x:sheetData>
   <x:pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>

</xml_diff>